<commit_message>
added vref DAC calc in excel file
</commit_message>
<xml_diff>
--- a/TrackAmplifier2.X/doc/Baudrate calc.xlsx
+++ b/TrackAmplifier2.X/doc/Baudrate calc.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Siebwalde-Source\trunk\SiebwaldeTrackAmplifier2.X\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Localdata\GIT_REPO\Siebwalde\TrackAmplifier2.X\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Fosc</t>
   </si>
@@ -40,15 +41,46 @@
   <si>
     <t>char delay in us</t>
   </si>
+  <si>
+    <t>Vsource+</t>
+  </si>
+  <si>
+    <t>Vsource-</t>
+  </si>
+  <si>
+    <t>Bit setting (0 - 32)</t>
+  </si>
+  <si>
+    <t>Rshunt</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Comp+ input</t>
+  </si>
+  <si>
+    <t>Comp- input</t>
+  </si>
+  <si>
+    <t>DAC Vout</t>
+  </si>
+  <si>
+    <t>Vsource+ can be externall ref (2.5V) or Vdd(5.0V) or Fvr(4.096V)</t>
+  </si>
+  <si>
+    <t>Gain INA326</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,8 +88,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,6 +109,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -80,19 +124,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -108,7 +157,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -406,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
@@ -3774,4 +3823,99 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="7"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4.0960000000000001</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7">
+        <f>((D3-D4)*(D5/32))+ D4</f>
+        <v>2.8159999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7">
+        <f>D6</f>
+        <v>2.8159999999999998</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7">
+        <f>G3*G5*G4+2.5</f>
+        <v>2.875</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated with resistor based ID calc
</commit_message>
<xml_diff>
--- a/TrackAmplifier2.X/doc/Baudrate calc.xlsx
+++ b/TrackAmplifier2.X/doc/Baudrate calc.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12795" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="12795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Fosc</t>
   </si>
@@ -71,6 +72,60 @@
   <si>
     <t>Gain INA326</t>
   </si>
+  <si>
+    <t>Rext</t>
+  </si>
+  <si>
+    <t>Volt ADC</t>
+  </si>
+  <si>
+    <t>resolution ADC [V/bit]</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>E24</t>
+  </si>
+  <si>
+    <t>E48</t>
+  </si>
+  <si>
+    <t>E96</t>
+  </si>
+  <si>
+    <t>E192</t>
+  </si>
+  <si>
+    <t>externall V = 5V</t>
+  </si>
+  <si>
+    <t>Bit val</t>
+  </si>
+  <si>
+    <t>delta Bit</t>
+  </si>
+  <si>
+    <t>Amp nr</t>
+  </si>
+  <si>
+    <t>E-48</t>
+  </si>
+  <si>
+    <t>Current on 5V ext</t>
+  </si>
+  <si>
+    <t>Total current required</t>
+  </si>
+  <si>
+    <t>delta mV</t>
+  </si>
 </sst>
 </file>
 
@@ -80,7 +135,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,8 +150,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,8 +182,14 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3FB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -123,12 +197,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -138,6 +307,38 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -3829,7 +4030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -3918,4 +4119,4207 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:U196"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="9"/>
+    <col min="7" max="7" width="15.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="2:21" ht="36.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="19">
+        <f>5/1024</f>
+        <v>4.8828125E-3</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3">
+        <f>SUM(J6:J55)</f>
+        <v>3.4904912669386383E-2</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="19"/>
+      <c r="O4" s="11">
+        <v>10</v>
+      </c>
+      <c r="P4" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>10</v>
+      </c>
+      <c r="R4" s="10">
+        <v>10</v>
+      </c>
+      <c r="S4" s="10">
+        <v>100</v>
+      </c>
+      <c r="T4" s="10">
+        <v>100</v>
+      </c>
+      <c r="U4" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="11">
+        <v>22</v>
+      </c>
+      <c r="P5" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>12</v>
+      </c>
+      <c r="R5" s="10">
+        <v>11</v>
+      </c>
+      <c r="S5" s="10">
+        <v>105</v>
+      </c>
+      <c r="T5" s="10">
+        <v>102</v>
+      </c>
+      <c r="U5" s="12">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B6" s="19">
+        <v>1</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20">
+        <f>S50</f>
+        <v>909</v>
+      </c>
+      <c r="E6" s="20">
+        <f>S51*10</f>
+        <v>9530</v>
+      </c>
+      <c r="F6" s="21">
+        <f>(5/($D6+$E6))*$D6</f>
+        <v>0.43538653127694221</v>
+      </c>
+      <c r="G6" s="20">
+        <f>ROUND(($F6/$G$3),0)</f>
+        <v>89</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21">
+        <v>440</v>
+      </c>
+      <c r="J6" s="19">
+        <f>5/($D6+$E6)</f>
+        <v>4.7897308171280774E-4</v>
+      </c>
+      <c r="O6" s="11">
+        <v>47</v>
+      </c>
+      <c r="P6" s="10">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>15</v>
+      </c>
+      <c r="R6" s="10">
+        <v>12</v>
+      </c>
+      <c r="S6" s="10">
+        <v>110</v>
+      </c>
+      <c r="T6" s="10">
+        <v>105</v>
+      </c>
+      <c r="U6" s="12">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B7" s="19">
+        <v>2</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20">
+        <v>953</v>
+      </c>
+      <c r="E7" s="20">
+        <f>S50*10</f>
+        <v>9090</v>
+      </c>
+      <c r="F7" s="21">
+        <f>(5/($D7+$E7))*$D7</f>
+        <v>0.4744598227621229</v>
+      </c>
+      <c r="G7" s="20">
+        <f>ROUND(($F7/$G$3),0)</f>
+        <v>97</v>
+      </c>
+      <c r="H7" s="20">
+        <f>G7-G6</f>
+        <v>8</v>
+      </c>
+      <c r="I7" s="21">
+        <f>(F7-F6)*1000</f>
+        <v>39.073291485180683</v>
+      </c>
+      <c r="J7" s="19">
+        <f t="shared" ref="J7:J55" si="0">5/($D7+$E7)</f>
+        <v>4.9785920541670818E-4</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="10">
+        <v>33</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>18</v>
+      </c>
+      <c r="R7" s="10">
+        <v>13</v>
+      </c>
+      <c r="S7" s="10">
+        <v>115</v>
+      </c>
+      <c r="T7" s="10">
+        <v>107</v>
+      </c>
+      <c r="U7" s="12">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B8" s="19">
+        <v>3</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20">
+        <f>S4*10</f>
+        <v>1000</v>
+      </c>
+      <c r="E8" s="20">
+        <f>S49*10</f>
+        <v>8660</v>
+      </c>
+      <c r="F8" s="21">
+        <f t="shared" ref="F8:F55" si="1">(5/($D8+$E8))*$D8</f>
+        <v>0.51759834368530022</v>
+      </c>
+      <c r="G8" s="20">
+        <f t="shared" ref="G8:G55" si="2">ROUND(($F8/$G$3),0)</f>
+        <v>106</v>
+      </c>
+      <c r="H8" s="20">
+        <f t="shared" ref="H8:H55" si="3">G8-G7</f>
+        <v>9</v>
+      </c>
+      <c r="I8" s="21">
+        <f t="shared" ref="I8:I55" si="4">(F8-F7)*1000</f>
+        <v>43.138520923177325</v>
+      </c>
+      <c r="J8" s="19">
+        <f t="shared" si="0"/>
+        <v>5.1759834368530024E-4</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10">
+        <v>47</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>22</v>
+      </c>
+      <c r="R8" s="10">
+        <v>15</v>
+      </c>
+      <c r="S8" s="10">
+        <v>121</v>
+      </c>
+      <c r="T8" s="10">
+        <v>110</v>
+      </c>
+      <c r="U8" s="12">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B9" s="19">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20">
+        <f>S5*10</f>
+        <v>1050</v>
+      </c>
+      <c r="E9" s="20">
+        <f>S48*10</f>
+        <v>8250</v>
+      </c>
+      <c r="F9" s="21">
+        <f t="shared" si="1"/>
+        <v>0.56451612903225812</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I9" s="21">
+        <f t="shared" si="4"/>
+        <v>46.917785346957899</v>
+      </c>
+      <c r="J9" s="19">
+        <f t="shared" si="0"/>
+        <v>5.3763440860215054E-4</v>
+      </c>
+      <c r="O9" s="11"/>
+      <c r="P9" s="10">
+        <v>68</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>27</v>
+      </c>
+      <c r="R9" s="10">
+        <v>16</v>
+      </c>
+      <c r="S9" s="10">
+        <v>127</v>
+      </c>
+      <c r="T9" s="10">
+        <v>113</v>
+      </c>
+      <c r="U9" s="12">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B10" s="19">
+        <v>5</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20">
+        <f>S6*10</f>
+        <v>1100</v>
+      </c>
+      <c r="E10" s="20">
+        <f>S47*10</f>
+        <v>7870</v>
+      </c>
+      <c r="F10" s="21">
+        <f t="shared" si="1"/>
+        <v>0.61315496098104794</v>
+      </c>
+      <c r="G10" s="20">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="H10" s="20">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I10" s="21">
+        <f t="shared" si="4"/>
+        <v>48.638831948789814</v>
+      </c>
+      <c r="J10" s="19">
+        <f t="shared" si="0"/>
+        <v>5.5741360089186175E-4</v>
+      </c>
+      <c r="O10" s="11"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10">
+        <v>33</v>
+      </c>
+      <c r="R10" s="10">
+        <v>18</v>
+      </c>
+      <c r="S10" s="10">
+        <v>133</v>
+      </c>
+      <c r="T10" s="10">
+        <v>115</v>
+      </c>
+      <c r="U10" s="12">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B11" s="19">
+        <v>6</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20">
+        <f>S7*10</f>
+        <v>1150</v>
+      </c>
+      <c r="E11" s="20">
+        <f>S46*10</f>
+        <v>7500</v>
+      </c>
+      <c r="F11" s="21">
+        <f t="shared" si="1"/>
+        <v>0.66473988439306364</v>
+      </c>
+      <c r="G11" s="20">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="H11" s="20">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I11" s="21">
+        <f t="shared" si="4"/>
+        <v>51.584923412015705</v>
+      </c>
+      <c r="J11" s="19">
+        <f t="shared" si="0"/>
+        <v>5.7803468208092489E-4</v>
+      </c>
+      <c r="O11" s="11"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10">
+        <v>39</v>
+      </c>
+      <c r="R11" s="10">
+        <v>20</v>
+      </c>
+      <c r="S11" s="10">
+        <v>140</v>
+      </c>
+      <c r="T11" s="10">
+        <v>118</v>
+      </c>
+      <c r="U11" s="12">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B12" s="19">
+        <v>7</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20">
+        <f>S8*10</f>
+        <v>1210</v>
+      </c>
+      <c r="E12" s="20">
+        <f>S45*10</f>
+        <v>7150</v>
+      </c>
+      <c r="F12" s="21">
+        <f t="shared" si="1"/>
+        <v>0.72368421052631571</v>
+      </c>
+      <c r="G12" s="20">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="H12" s="20">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="I12" s="21">
+        <f t="shared" si="4"/>
+        <v>58.944326133252069</v>
+      </c>
+      <c r="J12" s="19">
+        <f t="shared" si="0"/>
+        <v>5.9808612440191385E-4</v>
+      </c>
+      <c r="O12" s="11"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10">
+        <v>47</v>
+      </c>
+      <c r="R12" s="10">
+        <v>22</v>
+      </c>
+      <c r="S12" s="10">
+        <v>147</v>
+      </c>
+      <c r="T12" s="10">
+        <v>121</v>
+      </c>
+      <c r="U12" s="12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B13" s="19">
+        <v>8</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20">
+        <f>S9*10</f>
+        <v>1270</v>
+      </c>
+      <c r="E13" s="20">
+        <f>S44*10</f>
+        <v>6810</v>
+      </c>
+      <c r="F13" s="21">
+        <f t="shared" si="1"/>
+        <v>0.78589108910891092</v>
+      </c>
+      <c r="G13" s="20">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="H13" s="20">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="I13" s="21">
+        <f t="shared" si="4"/>
+        <v>62.206878582595216</v>
+      </c>
+      <c r="J13" s="19">
+        <f t="shared" si="0"/>
+        <v>6.1881188118811882E-4</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10">
+        <v>56</v>
+      </c>
+      <c r="R13" s="10">
+        <v>24</v>
+      </c>
+      <c r="S13" s="10">
+        <v>154</v>
+      </c>
+      <c r="T13" s="10">
+        <v>124</v>
+      </c>
+      <c r="U13" s="12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B14" s="19">
+        <v>9</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20">
+        <f>S10*10</f>
+        <v>1330</v>
+      </c>
+      <c r="E14" s="20">
+        <f>S43*10</f>
+        <v>6490</v>
+      </c>
+      <c r="F14" s="21">
+        <f t="shared" si="1"/>
+        <v>0.85038363171355502</v>
+      </c>
+      <c r="G14" s="20">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+      <c r="H14" s="20">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="I14" s="21">
+        <f t="shared" si="4"/>
+        <v>64.4925426046441</v>
+      </c>
+      <c r="J14" s="19">
+        <f t="shared" si="0"/>
+        <v>6.3938618925831207E-4</v>
+      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10">
+        <v>68</v>
+      </c>
+      <c r="R14" s="10">
+        <v>27</v>
+      </c>
+      <c r="S14" s="10">
+        <v>162</v>
+      </c>
+      <c r="T14" s="10">
+        <v>127</v>
+      </c>
+      <c r="U14" s="12">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B15" s="19">
+        <v>10</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20">
+        <f>S11*10</f>
+        <v>1400</v>
+      </c>
+      <c r="E15" s="20">
+        <f>S42*10</f>
+        <v>6190</v>
+      </c>
+      <c r="F15" s="21">
+        <f t="shared" si="1"/>
+        <v>0.92226613965744408</v>
+      </c>
+      <c r="G15" s="20">
+        <f t="shared" si="2"/>
+        <v>189</v>
+      </c>
+      <c r="H15" s="20">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="I15" s="21">
+        <f t="shared" si="4"/>
+        <v>71.882507943889067</v>
+      </c>
+      <c r="J15" s="19">
+        <f t="shared" si="0"/>
+        <v>6.5876152832674575E-4</v>
+      </c>
+      <c r="O15" s="11"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10">
+        <v>82</v>
+      </c>
+      <c r="R15" s="10">
+        <v>30</v>
+      </c>
+      <c r="S15" s="10">
+        <v>169</v>
+      </c>
+      <c r="T15" s="10">
+        <v>130</v>
+      </c>
+      <c r="U15" s="12">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B16" s="19">
+        <v>11</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20">
+        <f>S12*10</f>
+        <v>1470</v>
+      </c>
+      <c r="E16" s="20">
+        <f>S41*10</f>
+        <v>5900</v>
+      </c>
+      <c r="F16" s="21">
+        <f t="shared" si="1"/>
+        <v>0.99728629579375838</v>
+      </c>
+      <c r="G16" s="20">
+        <f t="shared" si="2"/>
+        <v>204</v>
+      </c>
+      <c r="H16" s="20">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="I16" s="21">
+        <f t="shared" si="4"/>
+        <v>75.020156136314299</v>
+      </c>
+      <c r="J16" s="19">
+        <f t="shared" si="0"/>
+        <v>6.7842605156037987E-4</v>
+      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10">
+        <v>33</v>
+      </c>
+      <c r="S16" s="10">
+        <v>178</v>
+      </c>
+      <c r="T16" s="10">
+        <v>133</v>
+      </c>
+      <c r="U16" s="12">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B17" s="19">
+        <v>12</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20">
+        <f>S13*10</f>
+        <v>1540</v>
+      </c>
+      <c r="E17" s="20">
+        <f>S40*10</f>
+        <v>5620</v>
+      </c>
+      <c r="F17" s="21">
+        <f t="shared" si="1"/>
+        <v>1.0754189944134078</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+      <c r="H17" s="20">
+        <f>G17-G16</f>
+        <v>16</v>
+      </c>
+      <c r="I17" s="21">
+        <f t="shared" si="4"/>
+        <v>78.132698619649446</v>
+      </c>
+      <c r="J17" s="19">
+        <f t="shared" si="0"/>
+        <v>6.9832402234636874E-4</v>
+      </c>
+      <c r="O17" s="11"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10">
+        <v>36</v>
+      </c>
+      <c r="S17" s="10">
+        <v>187</v>
+      </c>
+      <c r="T17" s="10">
+        <v>137</v>
+      </c>
+      <c r="U17" s="12">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B18" s="19">
+        <v>13</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20">
+        <f>S14*10</f>
+        <v>1620</v>
+      </c>
+      <c r="E18" s="20">
+        <f>S39*10</f>
+        <v>5360</v>
+      </c>
+      <c r="F18" s="21">
+        <f t="shared" si="1"/>
+        <v>1.1604584527220629</v>
+      </c>
+      <c r="G18" s="20">
+        <f t="shared" si="2"/>
+        <v>238</v>
+      </c>
+      <c r="H18" s="20">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="I18" s="21">
+        <f t="shared" si="4"/>
+        <v>85.039458308655114</v>
+      </c>
+      <c r="J18" s="19">
+        <f t="shared" si="0"/>
+        <v>7.1633237822349568E-4</v>
+      </c>
+      <c r="O18" s="11"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10">
+        <v>39</v>
+      </c>
+      <c r="S18" s="10">
+        <v>196</v>
+      </c>
+      <c r="T18" s="10">
+        <v>140</v>
+      </c>
+      <c r="U18" s="12">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B19" s="19">
+        <v>14</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20">
+        <f>S15*10</f>
+        <v>1690</v>
+      </c>
+      <c r="E19" s="20">
+        <f>S38*10</f>
+        <v>5110</v>
+      </c>
+      <c r="F19" s="21">
+        <f t="shared" si="1"/>
+        <v>1.2426470588235294</v>
+      </c>
+      <c r="G19" s="20">
+        <f t="shared" si="2"/>
+        <v>254</v>
+      </c>
+      <c r="H19" s="20">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I19" s="21">
+        <f t="shared" si="4"/>
+        <v>82.188606101466505</v>
+      </c>
+      <c r="J19" s="19">
+        <f t="shared" si="0"/>
+        <v>7.3529411764705881E-4</v>
+      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10">
+        <v>43</v>
+      </c>
+      <c r="S19" s="10">
+        <v>205</v>
+      </c>
+      <c r="T19" s="10">
+        <v>143</v>
+      </c>
+      <c r="U19" s="12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B20" s="19">
+        <v>15</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20">
+        <f>S16*10</f>
+        <v>1780</v>
+      </c>
+      <c r="E20" s="20">
+        <f>S37*10</f>
+        <v>4870</v>
+      </c>
+      <c r="F20" s="21">
+        <f t="shared" si="1"/>
+        <v>1.3383458646616542</v>
+      </c>
+      <c r="G20" s="20">
+        <f t="shared" si="2"/>
+        <v>274</v>
+      </c>
+      <c r="H20" s="20">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I20" s="21">
+        <f t="shared" si="4"/>
+        <v>95.698805838124741</v>
+      </c>
+      <c r="J20" s="19">
+        <f t="shared" si="0"/>
+        <v>7.5187969924812035E-4</v>
+      </c>
+      <c r="O20" s="11"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10">
+        <v>47</v>
+      </c>
+      <c r="S20" s="10">
+        <v>215</v>
+      </c>
+      <c r="T20" s="10">
+        <v>147</v>
+      </c>
+      <c r="U20" s="12">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B21" s="19">
+        <v>16</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20">
+        <f>S17*10</f>
+        <v>1870</v>
+      </c>
+      <c r="E21" s="20">
+        <f>S36*10</f>
+        <v>4640</v>
+      </c>
+      <c r="F21" s="21">
+        <f t="shared" si="1"/>
+        <v>1.4362519201228878</v>
+      </c>
+      <c r="G21" s="20">
+        <f t="shared" si="2"/>
+        <v>294</v>
+      </c>
+      <c r="H21" s="20">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I21" s="21">
+        <f t="shared" si="4"/>
+        <v>97.906055461233649</v>
+      </c>
+      <c r="J21" s="19">
+        <f t="shared" si="0"/>
+        <v>7.6804915514592934E-4</v>
+      </c>
+      <c r="O21" s="11"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10">
+        <v>51</v>
+      </c>
+      <c r="S21" s="10">
+        <v>226</v>
+      </c>
+      <c r="T21" s="10">
+        <v>150</v>
+      </c>
+      <c r="U21" s="12">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B22" s="19">
+        <v>17</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20">
+        <f>S18*10</f>
+        <v>1960</v>
+      </c>
+      <c r="E22" s="20">
+        <f>S35*10</f>
+        <v>4420</v>
+      </c>
+      <c r="F22" s="21">
+        <f t="shared" si="1"/>
+        <v>1.5360501567398119</v>
+      </c>
+      <c r="G22" s="20">
+        <f t="shared" si="2"/>
+        <v>315</v>
+      </c>
+      <c r="H22" s="20">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="I22" s="21">
+        <f t="shared" si="4"/>
+        <v>99.7982366169241</v>
+      </c>
+      <c r="J22" s="19">
+        <f t="shared" si="0"/>
+        <v>7.836990595611285E-4</v>
+      </c>
+      <c r="O22" s="11"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10">
+        <v>56</v>
+      </c>
+      <c r="S22" s="10">
+        <v>237</v>
+      </c>
+      <c r="T22" s="10">
+        <v>154</v>
+      </c>
+      <c r="U22" s="12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B23" s="19">
+        <v>18</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20">
+        <f>S19*10</f>
+        <v>2050</v>
+      </c>
+      <c r="E23" s="20">
+        <f>S34*10</f>
+        <v>4220</v>
+      </c>
+      <c r="F23" s="21">
+        <f t="shared" si="1"/>
+        <v>1.634768740031898</v>
+      </c>
+      <c r="G23" s="20">
+        <f t="shared" si="2"/>
+        <v>335</v>
+      </c>
+      <c r="H23" s="20">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I23" s="21">
+        <f t="shared" si="4"/>
+        <v>98.718583292086052</v>
+      </c>
+      <c r="J23" s="19">
+        <f t="shared" si="0"/>
+        <v>7.9744816586921851E-4</v>
+      </c>
+      <c r="O23" s="11"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10">
+        <v>62</v>
+      </c>
+      <c r="S23" s="10">
+        <v>249</v>
+      </c>
+      <c r="T23" s="10">
+        <v>158</v>
+      </c>
+      <c r="U23" s="12">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B24" s="19">
+        <v>19</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20">
+        <f>S20*10</f>
+        <v>2150</v>
+      </c>
+      <c r="E24" s="20">
+        <f>S33*10</f>
+        <v>4020</v>
+      </c>
+      <c r="F24" s="21">
+        <f t="shared" si="1"/>
+        <v>1.7423014586709886</v>
+      </c>
+      <c r="G24" s="20">
+        <f t="shared" si="2"/>
+        <v>357</v>
+      </c>
+      <c r="H24" s="20">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="I24" s="21">
+        <f t="shared" si="4"/>
+        <v>107.53271863909065</v>
+      </c>
+      <c r="J24" s="19">
+        <f t="shared" si="0"/>
+        <v>8.1037277147487841E-4</v>
+      </c>
+      <c r="O24" s="11"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10">
+        <v>68</v>
+      </c>
+      <c r="S24" s="10">
+        <v>261</v>
+      </c>
+      <c r="T24" s="10">
+        <v>162</v>
+      </c>
+      <c r="U24" s="12">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B25" s="19">
+        <v>20</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20">
+        <f>S21*10</f>
+        <v>2260</v>
+      </c>
+      <c r="E25" s="20">
+        <f>S32*10</f>
+        <v>3830</v>
+      </c>
+      <c r="F25" s="21">
+        <f t="shared" si="1"/>
+        <v>1.8555008210180624</v>
+      </c>
+      <c r="G25" s="20">
+        <f t="shared" si="2"/>
+        <v>380</v>
+      </c>
+      <c r="H25" s="20">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="I25" s="21">
+        <f t="shared" si="4"/>
+        <v>113.19936234707373</v>
+      </c>
+      <c r="J25" s="19">
+        <f t="shared" si="0"/>
+        <v>8.2101806239737272E-4</v>
+      </c>
+      <c r="O25" s="11"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10">
+        <v>75</v>
+      </c>
+      <c r="S25" s="10">
+        <v>274</v>
+      </c>
+      <c r="T25" s="10">
+        <v>165</v>
+      </c>
+      <c r="U25" s="12">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B26" s="19">
+        <v>21</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="20">
+        <f>S22*10</f>
+        <v>2370</v>
+      </c>
+      <c r="E26" s="20">
+        <f>S31*10</f>
+        <v>3650</v>
+      </c>
+      <c r="F26" s="21">
+        <f t="shared" si="1"/>
+        <v>1.9684385382059801</v>
+      </c>
+      <c r="G26" s="20">
+        <f t="shared" si="2"/>
+        <v>403</v>
+      </c>
+      <c r="H26" s="20">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="I26" s="21">
+        <f t="shared" si="4"/>
+        <v>112.93771718791778</v>
+      </c>
+      <c r="J26" s="19">
+        <f t="shared" si="0"/>
+        <v>8.3056478405315617E-4</v>
+      </c>
+      <c r="O26" s="11"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10">
+        <v>82</v>
+      </c>
+      <c r="S26" s="10">
+        <v>287</v>
+      </c>
+      <c r="T26" s="10">
+        <v>169</v>
+      </c>
+      <c r="U26" s="12">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B27" s="19">
+        <v>22</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20">
+        <f>S23*10</f>
+        <v>2490</v>
+      </c>
+      <c r="E27" s="20">
+        <f>S30*10</f>
+        <v>3480</v>
+      </c>
+      <c r="F27" s="21">
+        <f t="shared" si="1"/>
+        <v>2.0854271356783918</v>
+      </c>
+      <c r="G27" s="20">
+        <f t="shared" si="2"/>
+        <v>427</v>
+      </c>
+      <c r="H27" s="20">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="I27" s="21">
+        <f t="shared" si="4"/>
+        <v>116.98859747241164</v>
+      </c>
+      <c r="J27" s="19">
+        <f t="shared" si="0"/>
+        <v>8.375209380234506E-4</v>
+      </c>
+      <c r="O27" s="11"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10">
+        <v>91</v>
+      </c>
+      <c r="S27" s="10">
+        <v>301</v>
+      </c>
+      <c r="T27" s="10">
+        <v>174</v>
+      </c>
+      <c r="U27" s="12">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B28" s="19">
+        <v>23</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20">
+        <f>S24*10</f>
+        <v>2610</v>
+      </c>
+      <c r="E28" s="20">
+        <f>S29*10</f>
+        <v>3320</v>
+      </c>
+      <c r="F28" s="21">
+        <f t="shared" si="1"/>
+        <v>2.2006745362563236</v>
+      </c>
+      <c r="G28" s="20">
+        <f t="shared" si="2"/>
+        <v>451</v>
+      </c>
+      <c r="H28" s="20">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="21">
+        <f t="shared" si="4"/>
+        <v>115.24740057793181</v>
+      </c>
+      <c r="J28" s="19">
+        <f t="shared" si="0"/>
+        <v>8.4317032040472171E-4</v>
+      </c>
+      <c r="O28" s="11"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10">
+        <v>316</v>
+      </c>
+      <c r="T28" s="10">
+        <v>178</v>
+      </c>
+      <c r="U28" s="12">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B29" s="19">
+        <v>24</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20">
+        <f>S25*10</f>
+        <v>2740</v>
+      </c>
+      <c r="E29" s="20">
+        <f>S28*10</f>
+        <v>3160</v>
+      </c>
+      <c r="F29" s="21">
+        <f t="shared" si="1"/>
+        <v>2.3220338983050848</v>
+      </c>
+      <c r="G29" s="20">
+        <f t="shared" si="2"/>
+        <v>476</v>
+      </c>
+      <c r="H29" s="20">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="I29" s="21">
+        <f t="shared" si="4"/>
+        <v>121.35936204876118</v>
+      </c>
+      <c r="J29" s="19">
+        <f t="shared" si="0"/>
+        <v>8.4745762711864404E-4</v>
+      </c>
+      <c r="O29" s="11"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10">
+        <v>332</v>
+      </c>
+      <c r="T29" s="10">
+        <v>182</v>
+      </c>
+      <c r="U29" s="12">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B30" s="19">
+        <v>25</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20">
+        <f>S26*10</f>
+        <v>2870</v>
+      </c>
+      <c r="E30" s="20">
+        <f>S27*10</f>
+        <v>3010</v>
+      </c>
+      <c r="F30" s="21">
+        <f t="shared" si="1"/>
+        <v>2.4404761904761902</v>
+      </c>
+      <c r="G30" s="20">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="H30" s="20">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="I30" s="21">
+        <f t="shared" si="4"/>
+        <v>118.44229217110546</v>
+      </c>
+      <c r="J30" s="19">
+        <f t="shared" si="0"/>
+        <v>8.5034013605442174E-4</v>
+      </c>
+      <c r="O30" s="11"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10">
+        <v>348</v>
+      </c>
+      <c r="T30" s="10">
+        <v>187</v>
+      </c>
+      <c r="U30" s="12">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B31" s="19">
+        <v>26</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20">
+        <f>S27*10</f>
+        <v>3010</v>
+      </c>
+      <c r="E31" s="20">
+        <f>S26*10</f>
+        <v>2870</v>
+      </c>
+      <c r="F31" s="21">
+        <f t="shared" si="1"/>
+        <v>2.5595238095238093</v>
+      </c>
+      <c r="G31" s="20">
+        <f t="shared" si="2"/>
+        <v>524</v>
+      </c>
+      <c r="H31" s="20">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="I31" s="21">
+        <f t="shared" si="4"/>
+        <v>119.04761904761907</v>
+      </c>
+      <c r="J31" s="19">
+        <f t="shared" si="0"/>
+        <v>8.5034013605442174E-4</v>
+      </c>
+      <c r="O31" s="11"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10">
+        <v>365</v>
+      </c>
+      <c r="T31" s="10">
+        <v>191</v>
+      </c>
+      <c r="U31" s="12">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B32" s="19">
+        <v>27</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20">
+        <f>S28*10</f>
+        <v>3160</v>
+      </c>
+      <c r="E32" s="20">
+        <f>S25*10</f>
+        <v>2740</v>
+      </c>
+      <c r="F32" s="21">
+        <f t="shared" si="1"/>
+        <v>2.6779661016949152</v>
+      </c>
+      <c r="G32" s="20">
+        <f t="shared" si="2"/>
+        <v>548</v>
+      </c>
+      <c r="H32" s="20">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="I32" s="21">
+        <f t="shared" si="4"/>
+        <v>118.44229217110592</v>
+      </c>
+      <c r="J32" s="19">
+        <f t="shared" si="0"/>
+        <v>8.4745762711864404E-4</v>
+      </c>
+      <c r="O32" s="11"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10">
+        <v>383</v>
+      </c>
+      <c r="T32" s="10">
+        <v>196</v>
+      </c>
+      <c r="U32" s="12">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B33" s="19">
+        <v>28</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20">
+        <f>S29*10</f>
+        <v>3320</v>
+      </c>
+      <c r="E33" s="20">
+        <f>S24*10</f>
+        <v>2610</v>
+      </c>
+      <c r="F33" s="21">
+        <f t="shared" si="1"/>
+        <v>2.799325463743676</v>
+      </c>
+      <c r="G33" s="20">
+        <f t="shared" si="2"/>
+        <v>573</v>
+      </c>
+      <c r="H33" s="20">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="I33" s="21">
+        <f t="shared" si="4"/>
+        <v>121.35936204876074</v>
+      </c>
+      <c r="J33" s="19">
+        <f t="shared" si="0"/>
+        <v>8.4317032040472171E-4</v>
+      </c>
+      <c r="O33" s="11"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10">
+        <v>402</v>
+      </c>
+      <c r="T33" s="10">
+        <v>200</v>
+      </c>
+      <c r="U33" s="12">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B34" s="19">
+        <v>29</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20">
+        <f>S30*10</f>
+        <v>3480</v>
+      </c>
+      <c r="E34" s="20">
+        <f>S23*10</f>
+        <v>2490</v>
+      </c>
+      <c r="F34" s="21">
+        <f t="shared" si="1"/>
+        <v>2.9145728643216082</v>
+      </c>
+      <c r="G34" s="20">
+        <f t="shared" si="2"/>
+        <v>597</v>
+      </c>
+      <c r="H34" s="20">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="I34" s="21">
+        <f t="shared" si="4"/>
+        <v>115.24740057793225</v>
+      </c>
+      <c r="J34" s="19">
+        <f t="shared" si="0"/>
+        <v>8.375209380234506E-4</v>
+      </c>
+      <c r="O34" s="11"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10">
+        <v>422</v>
+      </c>
+      <c r="T34" s="10">
+        <v>205</v>
+      </c>
+      <c r="U34" s="12">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B35" s="19">
+        <v>30</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20">
+        <f>S31*10</f>
+        <v>3650</v>
+      </c>
+      <c r="E35" s="20">
+        <f>S22*10</f>
+        <v>2370</v>
+      </c>
+      <c r="F35" s="21">
+        <f t="shared" si="1"/>
+        <v>3.0315614617940199</v>
+      </c>
+      <c r="G35" s="20">
+        <f t="shared" si="2"/>
+        <v>621</v>
+      </c>
+      <c r="H35" s="20">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="I35" s="21">
+        <f t="shared" si="4"/>
+        <v>116.98859747241164</v>
+      </c>
+      <c r="J35" s="19">
+        <f t="shared" si="0"/>
+        <v>8.3056478405315617E-4</v>
+      </c>
+      <c r="O35" s="11"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10">
+        <v>442</v>
+      </c>
+      <c r="T35" s="10">
+        <v>210</v>
+      </c>
+      <c r="U35" s="12">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B36" s="19">
+        <v>31</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20">
+        <f>S32*10</f>
+        <v>3830</v>
+      </c>
+      <c r="E36" s="20">
+        <f>S21*10</f>
+        <v>2260</v>
+      </c>
+      <c r="F36" s="21">
+        <f t="shared" si="1"/>
+        <v>3.1444991789819374</v>
+      </c>
+      <c r="G36" s="20">
+        <f t="shared" si="2"/>
+        <v>644</v>
+      </c>
+      <c r="H36" s="20">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="I36" s="21">
+        <f t="shared" si="4"/>
+        <v>112.93771718791757</v>
+      </c>
+      <c r="J36" s="19">
+        <f t="shared" si="0"/>
+        <v>8.2101806239737272E-4</v>
+      </c>
+      <c r="O36" s="11"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10">
+        <v>464</v>
+      </c>
+      <c r="T36" s="10">
+        <v>215</v>
+      </c>
+      <c r="U36" s="12">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B37" s="19">
+        <v>32</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20">
+        <f>S33*10</f>
+        <v>4020</v>
+      </c>
+      <c r="E37" s="20">
+        <f>S20*10</f>
+        <v>2150</v>
+      </c>
+      <c r="F37" s="21">
+        <f t="shared" si="1"/>
+        <v>3.2576985413290114</v>
+      </c>
+      <c r="G37" s="20">
+        <f t="shared" si="2"/>
+        <v>667</v>
+      </c>
+      <c r="H37" s="20">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="I37" s="21">
+        <f t="shared" si="4"/>
+        <v>113.19936234707396</v>
+      </c>
+      <c r="J37" s="19">
+        <f t="shared" si="0"/>
+        <v>8.1037277147487841E-4</v>
+      </c>
+      <c r="O37" s="11"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10">
+        <v>487</v>
+      </c>
+      <c r="T37" s="10">
+        <v>221</v>
+      </c>
+      <c r="U37" s="12">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B38" s="19">
+        <v>33</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20">
+        <f>S34*10</f>
+        <v>4220</v>
+      </c>
+      <c r="E38" s="20">
+        <f>S19*10</f>
+        <v>2050</v>
+      </c>
+      <c r="F38" s="21">
+        <f t="shared" si="1"/>
+        <v>3.3652312599681022</v>
+      </c>
+      <c r="G38" s="20">
+        <f t="shared" si="2"/>
+        <v>689</v>
+      </c>
+      <c r="H38" s="20">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="I38" s="21">
+        <f t="shared" si="4"/>
+        <v>107.53271863909086</v>
+      </c>
+      <c r="J38" s="19">
+        <f t="shared" si="0"/>
+        <v>7.9744816586921851E-4</v>
+      </c>
+      <c r="O38" s="11"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10">
+        <v>511</v>
+      </c>
+      <c r="T38" s="10">
+        <v>226</v>
+      </c>
+      <c r="U38" s="12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B39" s="19">
+        <v>34</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="20">
+        <f>S35*10</f>
+        <v>4420</v>
+      </c>
+      <c r="E39" s="20">
+        <f>S18*10</f>
+        <v>1960</v>
+      </c>
+      <c r="F39" s="21">
+        <f t="shared" si="1"/>
+        <v>3.4639498432601878</v>
+      </c>
+      <c r="G39" s="20">
+        <f t="shared" si="2"/>
+        <v>709</v>
+      </c>
+      <c r="H39" s="20">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I39" s="21">
+        <f t="shared" si="4"/>
+        <v>98.718583292085611</v>
+      </c>
+      <c r="J39" s="19">
+        <f t="shared" si="0"/>
+        <v>7.836990595611285E-4</v>
+      </c>
+      <c r="O39" s="11"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10">
+        <v>536</v>
+      </c>
+      <c r="T39" s="10">
+        <v>232</v>
+      </c>
+      <c r="U39" s="12">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B40" s="19">
+        <v>35</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20">
+        <f>S36*10</f>
+        <v>4640</v>
+      </c>
+      <c r="E40" s="20">
+        <f>S17*10</f>
+        <v>1870</v>
+      </c>
+      <c r="F40" s="21">
+        <f t="shared" si="1"/>
+        <v>3.563748079877112</v>
+      </c>
+      <c r="G40" s="20">
+        <f t="shared" si="2"/>
+        <v>730</v>
+      </c>
+      <c r="H40" s="20">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="I40" s="21">
+        <f t="shared" si="4"/>
+        <v>99.7982366169241</v>
+      </c>
+      <c r="J40" s="19">
+        <f t="shared" si="0"/>
+        <v>7.6804915514592934E-4</v>
+      </c>
+      <c r="O40" s="11"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10">
+        <v>562</v>
+      </c>
+      <c r="T40" s="10">
+        <v>237</v>
+      </c>
+      <c r="U40" s="12">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B41" s="19">
+        <v>36</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="20">
+        <f>S37*10</f>
+        <v>4870</v>
+      </c>
+      <c r="E41" s="20">
+        <f>S16*10</f>
+        <v>1780</v>
+      </c>
+      <c r="F41" s="21">
+        <f t="shared" si="1"/>
+        <v>3.6616541353383463</v>
+      </c>
+      <c r="G41" s="20">
+        <f t="shared" si="2"/>
+        <v>750</v>
+      </c>
+      <c r="H41" s="20">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I41" s="21">
+        <f t="shared" si="4"/>
+        <v>97.906055461234317</v>
+      </c>
+      <c r="J41" s="19">
+        <f t="shared" si="0"/>
+        <v>7.5187969924812035E-4</v>
+      </c>
+      <c r="O41" s="11"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10">
+        <v>590</v>
+      </c>
+      <c r="T41" s="10">
+        <v>243</v>
+      </c>
+      <c r="U41" s="12">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B42" s="19">
+        <v>37</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20">
+        <f>S38*10</f>
+        <v>5110</v>
+      </c>
+      <c r="E42" s="20">
+        <f>S15*10</f>
+        <v>1690</v>
+      </c>
+      <c r="F42" s="21">
+        <f t="shared" si="1"/>
+        <v>3.7573529411764706</v>
+      </c>
+      <c r="G42" s="20">
+        <f t="shared" si="2"/>
+        <v>770</v>
+      </c>
+      <c r="H42" s="20">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I42" s="21">
+        <f t="shared" si="4"/>
+        <v>95.698805838124287</v>
+      </c>
+      <c r="J42" s="19">
+        <f t="shared" si="0"/>
+        <v>7.3529411764705881E-4</v>
+      </c>
+      <c r="O42" s="11"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10">
+        <v>619</v>
+      </c>
+      <c r="T42" s="10">
+        <v>249</v>
+      </c>
+      <c r="U42" s="12">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B43" s="19">
+        <v>38</v>
+      </c>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20">
+        <f>S39*10</f>
+        <v>5360</v>
+      </c>
+      <c r="E43" s="20">
+        <f>S14*10</f>
+        <v>1620</v>
+      </c>
+      <c r="F43" s="21">
+        <f t="shared" si="1"/>
+        <v>3.8395415472779368</v>
+      </c>
+      <c r="G43" s="20">
+        <f t="shared" si="2"/>
+        <v>786</v>
+      </c>
+      <c r="H43" s="20">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I43" s="21">
+        <f t="shared" si="4"/>
+        <v>82.188606101466277</v>
+      </c>
+      <c r="J43" s="19">
+        <f t="shared" si="0"/>
+        <v>7.1633237822349568E-4</v>
+      </c>
+      <c r="O43" s="11"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10">
+        <v>649</v>
+      </c>
+      <c r="T43" s="10">
+        <v>255</v>
+      </c>
+      <c r="U43" s="12">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B44" s="19">
+        <v>39</v>
+      </c>
+      <c r="C44" s="19"/>
+      <c r="D44" s="20">
+        <f>S40*10</f>
+        <v>5620</v>
+      </c>
+      <c r="E44" s="20">
+        <f>S13*10</f>
+        <v>1540</v>
+      </c>
+      <c r="F44" s="21">
+        <f t="shared" si="1"/>
+        <v>3.9245810055865924</v>
+      </c>
+      <c r="G44" s="20">
+        <f t="shared" si="2"/>
+        <v>804</v>
+      </c>
+      <c r="H44" s="20">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="I44" s="21">
+        <f t="shared" si="4"/>
+        <v>85.039458308655554</v>
+      </c>
+      <c r="J44" s="19">
+        <f t="shared" si="0"/>
+        <v>6.9832402234636874E-4</v>
+      </c>
+      <c r="O44" s="11"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10">
+        <v>681</v>
+      </c>
+      <c r="T44" s="10">
+        <v>261</v>
+      </c>
+      <c r="U44" s="12">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B45" s="19">
+        <v>40</v>
+      </c>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20">
+        <f>S41*10</f>
+        <v>5900</v>
+      </c>
+      <c r="E45" s="20">
+        <f>S12*10</f>
+        <v>1470</v>
+      </c>
+      <c r="F45" s="21">
+        <f t="shared" si="1"/>
+        <v>4.0027137042062408</v>
+      </c>
+      <c r="G45" s="20">
+        <f t="shared" si="2"/>
+        <v>820</v>
+      </c>
+      <c r="H45" s="20">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="I45" s="21">
+        <f t="shared" si="4"/>
+        <v>78.132698619648437</v>
+      </c>
+      <c r="J45" s="19">
+        <f t="shared" si="0"/>
+        <v>6.7842605156037987E-4</v>
+      </c>
+      <c r="O45" s="11"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10">
+        <v>715</v>
+      </c>
+      <c r="T45" s="10">
+        <v>267</v>
+      </c>
+      <c r="U45" s="12">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B46" s="19">
+        <v>41</v>
+      </c>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20">
+        <f>S42*10</f>
+        <v>6190</v>
+      </c>
+      <c r="E46" s="20">
+        <f>S11*10</f>
+        <v>1400</v>
+      </c>
+      <c r="F46" s="21">
+        <f t="shared" si="1"/>
+        <v>4.0777338603425566</v>
+      </c>
+      <c r="G46" s="20">
+        <f t="shared" si="2"/>
+        <v>835</v>
+      </c>
+      <c r="H46" s="20">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="I46" s="21">
+        <f t="shared" si="4"/>
+        <v>75.020156136315734</v>
+      </c>
+      <c r="J46" s="19">
+        <f t="shared" si="0"/>
+        <v>6.5876152832674575E-4</v>
+      </c>
+      <c r="O46" s="11"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10">
+        <v>750</v>
+      </c>
+      <c r="T46" s="10">
+        <v>274</v>
+      </c>
+      <c r="U46" s="12">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B47" s="19">
+        <v>42</v>
+      </c>
+      <c r="C47" s="19"/>
+      <c r="D47" s="20">
+        <f>S43*10</f>
+        <v>6490</v>
+      </c>
+      <c r="E47" s="20">
+        <f>S10*10</f>
+        <v>1330</v>
+      </c>
+      <c r="F47" s="21">
+        <f t="shared" si="1"/>
+        <v>4.1496163682864458</v>
+      </c>
+      <c r="G47" s="20">
+        <f t="shared" si="2"/>
+        <v>850</v>
+      </c>
+      <c r="H47" s="20">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="I47" s="21">
+        <f t="shared" si="4"/>
+        <v>71.882507943889181</v>
+      </c>
+      <c r="J47" s="19">
+        <f t="shared" si="0"/>
+        <v>6.3938618925831207E-4</v>
+      </c>
+      <c r="O47" s="11"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+      <c r="S47" s="10">
+        <v>787</v>
+      </c>
+      <c r="T47" s="10">
+        <v>280</v>
+      </c>
+      <c r="U47" s="12">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B48" s="19">
+        <v>43</v>
+      </c>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20">
+        <f>S44*10</f>
+        <v>6810</v>
+      </c>
+      <c r="E48" s="20">
+        <f>S9*10</f>
+        <v>1270</v>
+      </c>
+      <c r="F48" s="21">
+        <f t="shared" si="1"/>
+        <v>4.2141089108910892</v>
+      </c>
+      <c r="G48" s="20">
+        <f t="shared" si="2"/>
+        <v>863</v>
+      </c>
+      <c r="H48" s="20">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="I48" s="21">
+        <f t="shared" si="4"/>
+        <v>64.492542604643432</v>
+      </c>
+      <c r="J48" s="19">
+        <f t="shared" si="0"/>
+        <v>6.1881188118811882E-4</v>
+      </c>
+      <c r="O48" s="11"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+      <c r="S48" s="10">
+        <v>825</v>
+      </c>
+      <c r="T48" s="10">
+        <v>287</v>
+      </c>
+      <c r="U48" s="12">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B49" s="19">
+        <v>44</v>
+      </c>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20">
+        <f>S45*10</f>
+        <v>7150</v>
+      </c>
+      <c r="E49" s="20">
+        <f>S8*10</f>
+        <v>1210</v>
+      </c>
+      <c r="F49" s="21">
+        <f t="shared" si="1"/>
+        <v>4.2763157894736841</v>
+      </c>
+      <c r="G49" s="20">
+        <f t="shared" si="2"/>
+        <v>876</v>
+      </c>
+      <c r="H49" s="20">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="I49" s="21">
+        <f t="shared" si="4"/>
+        <v>62.206878582594882</v>
+      </c>
+      <c r="J49" s="19">
+        <f t="shared" si="0"/>
+        <v>5.9808612440191385E-4</v>
+      </c>
+      <c r="O49" s="11"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+      <c r="R49" s="10"/>
+      <c r="S49" s="10">
+        <v>866</v>
+      </c>
+      <c r="T49" s="10">
+        <v>294</v>
+      </c>
+      <c r="U49" s="12">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B50" s="19">
+        <v>45</v>
+      </c>
+      <c r="C50" s="19"/>
+      <c r="D50" s="20">
+        <f>S46*10</f>
+        <v>7500</v>
+      </c>
+      <c r="E50" s="20">
+        <f>S7*10</f>
+        <v>1150</v>
+      </c>
+      <c r="F50" s="21">
+        <f t="shared" si="1"/>
+        <v>4.3352601156069364</v>
+      </c>
+      <c r="G50" s="20">
+        <f t="shared" si="2"/>
+        <v>888</v>
+      </c>
+      <c r="H50" s="20">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="I50" s="21">
+        <f t="shared" si="4"/>
+        <v>58.944326133252289</v>
+      </c>
+      <c r="J50" s="19">
+        <f t="shared" si="0"/>
+        <v>5.7803468208092489E-4</v>
+      </c>
+      <c r="O50" s="11"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10">
+        <v>909</v>
+      </c>
+      <c r="T50" s="10">
+        <v>301</v>
+      </c>
+      <c r="U50" s="12">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B51" s="19">
+        <v>46</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="20">
+        <f>S47*10</f>
+        <v>7870</v>
+      </c>
+      <c r="E51" s="20">
+        <f>S6*10</f>
+        <v>1100</v>
+      </c>
+      <c r="F51" s="21">
+        <f t="shared" si="1"/>
+        <v>4.3868450390189517</v>
+      </c>
+      <c r="G51" s="20">
+        <f t="shared" si="2"/>
+        <v>898</v>
+      </c>
+      <c r="H51" s="20">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I51" s="21">
+        <f t="shared" si="4"/>
+        <v>51.584923412015371</v>
+      </c>
+      <c r="J51" s="19">
+        <f t="shared" si="0"/>
+        <v>5.5741360089186175E-4</v>
+      </c>
+      <c r="O51" s="11"/>
+      <c r="P51" s="10"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+      <c r="S51" s="10">
+        <v>953</v>
+      </c>
+      <c r="T51" s="10">
+        <v>309</v>
+      </c>
+      <c r="U51" s="12">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B52" s="19">
+        <v>47</v>
+      </c>
+      <c r="C52" s="19"/>
+      <c r="D52" s="20">
+        <f>S48*10</f>
+        <v>8250</v>
+      </c>
+      <c r="E52" s="20">
+        <f>S5*10</f>
+        <v>1050</v>
+      </c>
+      <c r="F52" s="21">
+        <f t="shared" si="1"/>
+        <v>4.435483870967742</v>
+      </c>
+      <c r="G52" s="20">
+        <f t="shared" si="2"/>
+        <v>908</v>
+      </c>
+      <c r="H52" s="20">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I52" s="21">
+        <f t="shared" si="4"/>
+        <v>48.638831948790262</v>
+      </c>
+      <c r="J52" s="19">
+        <f t="shared" si="0"/>
+        <v>5.3763440860215054E-4</v>
+      </c>
+      <c r="O52" s="11"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+      <c r="S52" s="10"/>
+      <c r="T52" s="10">
+        <v>316</v>
+      </c>
+      <c r="U52" s="12">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B53" s="19">
+        <v>48</v>
+      </c>
+      <c r="C53" s="19"/>
+      <c r="D53" s="20">
+        <f>S49*10</f>
+        <v>8660</v>
+      </c>
+      <c r="E53" s="20">
+        <f>S4*10</f>
+        <v>1000</v>
+      </c>
+      <c r="F53" s="21">
+        <f t="shared" si="1"/>
+        <v>4.4824016563146998</v>
+      </c>
+      <c r="G53" s="20">
+        <f t="shared" si="2"/>
+        <v>918</v>
+      </c>
+      <c r="H53" s="20">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="I53" s="21">
+        <f t="shared" si="4"/>
+        <v>46.917785346957785</v>
+      </c>
+      <c r="J53" s="19">
+        <f t="shared" si="0"/>
+        <v>5.1759834368530024E-4</v>
+      </c>
+      <c r="O53" s="11"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+      <c r="S53" s="10"/>
+      <c r="T53" s="10">
+        <v>324</v>
+      </c>
+      <c r="U53" s="12">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B54" s="19">
+        <v>49</v>
+      </c>
+      <c r="C54" s="19"/>
+      <c r="D54" s="20">
+        <f>S50*10</f>
+        <v>9090</v>
+      </c>
+      <c r="E54" s="20">
+        <f>S51</f>
+        <v>953</v>
+      </c>
+      <c r="F54" s="21">
+        <f t="shared" si="1"/>
+        <v>4.5255401772378772</v>
+      </c>
+      <c r="G54" s="20">
+        <f t="shared" si="2"/>
+        <v>927</v>
+      </c>
+      <c r="H54" s="20">
+        <f>G54-G53</f>
+        <v>9</v>
+      </c>
+      <c r="I54" s="21">
+        <f t="shared" si="4"/>
+        <v>43.138520923177381</v>
+      </c>
+      <c r="J54" s="19">
+        <f t="shared" si="0"/>
+        <v>4.9785920541670818E-4</v>
+      </c>
+      <c r="O54" s="11"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
+      <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="10">
+        <v>332</v>
+      </c>
+      <c r="U54" s="12">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="B55" s="19">
+        <v>50</v>
+      </c>
+      <c r="C55" s="19"/>
+      <c r="D55" s="20">
+        <f>S51*10</f>
+        <v>9530</v>
+      </c>
+      <c r="E55" s="20">
+        <f>S50</f>
+        <v>909</v>
+      </c>
+      <c r="F55" s="21">
+        <f t="shared" si="1"/>
+        <v>4.5646134687230582</v>
+      </c>
+      <c r="G55" s="20">
+        <f t="shared" si="2"/>
+        <v>935</v>
+      </c>
+      <c r="H55" s="20">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="I55" s="21">
+        <f t="shared" si="4"/>
+        <v>39.073291485181016</v>
+      </c>
+      <c r="J55" s="19">
+        <f t="shared" si="0"/>
+        <v>4.7897308171280774E-4</v>
+      </c>
+      <c r="O55" s="11"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
+      <c r="R55" s="10"/>
+      <c r="S55" s="10"/>
+      <c r="T55" s="10">
+        <v>340</v>
+      </c>
+      <c r="U55" s="12">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O56" s="11"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="10"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10">
+        <v>348</v>
+      </c>
+      <c r="U56" s="12">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O57" s="11"/>
+      <c r="P57" s="10"/>
+      <c r="Q57" s="10"/>
+      <c r="R57" s="10"/>
+      <c r="S57" s="10"/>
+      <c r="T57" s="10">
+        <v>357</v>
+      </c>
+      <c r="U57" s="12">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O58" s="11"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="10">
+        <v>365</v>
+      </c>
+      <c r="U58" s="12">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O59" s="11"/>
+      <c r="P59" s="10"/>
+      <c r="Q59" s="10"/>
+      <c r="R59" s="10"/>
+      <c r="S59" s="10"/>
+      <c r="T59" s="10">
+        <v>374</v>
+      </c>
+      <c r="U59" s="12">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O60" s="11"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
+      <c r="R60" s="10"/>
+      <c r="S60" s="10"/>
+      <c r="T60" s="10">
+        <v>383</v>
+      </c>
+      <c r="U60" s="12">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O61" s="11"/>
+      <c r="P61" s="10"/>
+      <c r="Q61" s="10"/>
+      <c r="R61" s="10"/>
+      <c r="S61" s="10"/>
+      <c r="T61" s="10">
+        <v>392</v>
+      </c>
+      <c r="U61" s="12">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="62" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O62" s="11"/>
+      <c r="P62" s="10"/>
+      <c r="Q62" s="10"/>
+      <c r="R62" s="10"/>
+      <c r="S62" s="10"/>
+      <c r="T62" s="10">
+        <v>402</v>
+      </c>
+      <c r="U62" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O63" s="11"/>
+      <c r="P63" s="10"/>
+      <c r="Q63" s="10"/>
+      <c r="R63" s="10"/>
+      <c r="S63" s="10"/>
+      <c r="T63" s="10">
+        <v>412</v>
+      </c>
+      <c r="U63" s="12">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O64" s="11"/>
+      <c r="P64" s="10"/>
+      <c r="Q64" s="10"/>
+      <c r="R64" s="10"/>
+      <c r="S64" s="10"/>
+      <c r="T64" s="10">
+        <v>422</v>
+      </c>
+      <c r="U64" s="12">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O65" s="11"/>
+      <c r="P65" s="10"/>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10">
+        <v>432</v>
+      </c>
+      <c r="U65" s="12">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="66" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O66" s="11"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10">
+        <v>442</v>
+      </c>
+      <c r="U66" s="12">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="67" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O67" s="11"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10">
+        <v>453</v>
+      </c>
+      <c r="U67" s="12">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="68" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O68" s="11"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="10"/>
+      <c r="R68" s="10"/>
+      <c r="S68" s="10"/>
+      <c r="T68" s="10">
+        <v>464</v>
+      </c>
+      <c r="U68" s="12">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O69" s="11"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10">
+        <v>475</v>
+      </c>
+      <c r="U69" s="12">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="70" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O70" s="11"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="10"/>
+      <c r="S70" s="10"/>
+      <c r="T70" s="10">
+        <v>487</v>
+      </c>
+      <c r="U70" s="12">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="71" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O71" s="11"/>
+      <c r="P71" s="10"/>
+      <c r="Q71" s="10"/>
+      <c r="R71" s="10"/>
+      <c r="S71" s="10"/>
+      <c r="T71" s="10">
+        <v>499</v>
+      </c>
+      <c r="U71" s="12">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O72" s="11"/>
+      <c r="P72" s="10"/>
+      <c r="Q72" s="10"/>
+      <c r="R72" s="10"/>
+      <c r="S72" s="10"/>
+      <c r="T72" s="10">
+        <v>511</v>
+      </c>
+      <c r="U72" s="12">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O73" s="11"/>
+      <c r="P73" s="10"/>
+      <c r="Q73" s="10"/>
+      <c r="R73" s="10"/>
+      <c r="S73" s="10"/>
+      <c r="T73" s="10">
+        <v>523</v>
+      </c>
+      <c r="U73" s="12">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="74" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O74" s="11"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="10">
+        <v>536</v>
+      </c>
+      <c r="U74" s="12">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="75" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O75" s="11"/>
+      <c r="P75" s="10"/>
+      <c r="Q75" s="10"/>
+      <c r="R75" s="10"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10">
+        <v>549</v>
+      </c>
+      <c r="U75" s="12">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="76" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O76" s="11"/>
+      <c r="P76" s="10"/>
+      <c r="Q76" s="10"/>
+      <c r="R76" s="10"/>
+      <c r="S76" s="10"/>
+      <c r="T76" s="10">
+        <v>562</v>
+      </c>
+      <c r="U76" s="12">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="77" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O77" s="11"/>
+      <c r="P77" s="10"/>
+      <c r="Q77" s="10"/>
+      <c r="R77" s="10"/>
+      <c r="S77" s="10"/>
+      <c r="T77" s="10">
+        <v>576</v>
+      </c>
+      <c r="U77" s="12">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O78" s="11"/>
+      <c r="P78" s="10"/>
+      <c r="Q78" s="10"/>
+      <c r="R78" s="10"/>
+      <c r="S78" s="10"/>
+      <c r="T78" s="10">
+        <v>590</v>
+      </c>
+      <c r="U78" s="12">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="79" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O79" s="11"/>
+      <c r="P79" s="10"/>
+      <c r="Q79" s="10"/>
+      <c r="R79" s="10"/>
+      <c r="S79" s="10"/>
+      <c r="T79" s="10">
+        <v>604</v>
+      </c>
+      <c r="U79" s="12">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="80" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O80" s="11"/>
+      <c r="P80" s="10"/>
+      <c r="Q80" s="10"/>
+      <c r="R80" s="10"/>
+      <c r="S80" s="10"/>
+      <c r="T80" s="10">
+        <v>619</v>
+      </c>
+      <c r="U80" s="12">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="81" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O81" s="11"/>
+      <c r="P81" s="10"/>
+      <c r="Q81" s="10"/>
+      <c r="R81" s="10"/>
+      <c r="S81" s="10"/>
+      <c r="T81" s="10">
+        <v>634</v>
+      </c>
+      <c r="U81" s="12">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="82" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O82" s="11"/>
+      <c r="P82" s="10"/>
+      <c r="Q82" s="10"/>
+      <c r="R82" s="10"/>
+      <c r="S82" s="10"/>
+      <c r="T82" s="10">
+        <v>649</v>
+      </c>
+      <c r="U82" s="12">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O83" s="11"/>
+      <c r="P83" s="10"/>
+      <c r="Q83" s="10"/>
+      <c r="R83" s="10"/>
+      <c r="S83" s="10"/>
+      <c r="T83" s="10">
+        <v>665</v>
+      </c>
+      <c r="U83" s="12">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O84" s="11"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="10"/>
+      <c r="R84" s="10"/>
+      <c r="S84" s="10"/>
+      <c r="T84" s="10">
+        <v>681</v>
+      </c>
+      <c r="U84" s="12">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O85" s="11"/>
+      <c r="P85" s="10"/>
+      <c r="Q85" s="10"/>
+      <c r="R85" s="10"/>
+      <c r="S85" s="10"/>
+      <c r="T85" s="10">
+        <v>698</v>
+      </c>
+      <c r="U85" s="12">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="86" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O86" s="11"/>
+      <c r="P86" s="10"/>
+      <c r="Q86" s="10"/>
+      <c r="R86" s="10"/>
+      <c r="S86" s="10"/>
+      <c r="T86" s="10">
+        <v>715</v>
+      </c>
+      <c r="U86" s="12">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O87" s="11"/>
+      <c r="P87" s="10"/>
+      <c r="Q87" s="10"/>
+      <c r="R87" s="10"/>
+      <c r="S87" s="10"/>
+      <c r="T87" s="10">
+        <v>732</v>
+      </c>
+      <c r="U87" s="12">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="88" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O88" s="11"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="10"/>
+      <c r="R88" s="10"/>
+      <c r="S88" s="10"/>
+      <c r="T88" s="10">
+        <v>750</v>
+      </c>
+      <c r="U88" s="12">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="89" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O89" s="11"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10">
+        <v>768</v>
+      </c>
+      <c r="U89" s="12">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="90" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O90" s="11"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10">
+        <v>787</v>
+      </c>
+      <c r="U90" s="12">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="91" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O91" s="11"/>
+      <c r="P91" s="10"/>
+      <c r="Q91" s="10"/>
+      <c r="R91" s="10"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="10">
+        <v>806</v>
+      </c>
+      <c r="U91" s="12">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="92" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O92" s="11"/>
+      <c r="P92" s="10"/>
+      <c r="Q92" s="10"/>
+      <c r="R92" s="10"/>
+      <c r="S92" s="10"/>
+      <c r="T92" s="10">
+        <v>825</v>
+      </c>
+      <c r="U92" s="12">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="93" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O93" s="11"/>
+      <c r="P93" s="10"/>
+      <c r="Q93" s="10"/>
+      <c r="R93" s="10"/>
+      <c r="S93" s="10"/>
+      <c r="T93" s="10">
+        <v>845</v>
+      </c>
+      <c r="U93" s="12">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="94" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O94" s="11"/>
+      <c r="P94" s="10"/>
+      <c r="Q94" s="10"/>
+      <c r="R94" s="10"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10">
+        <v>866</v>
+      </c>
+      <c r="U94" s="12">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="95" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O95" s="11"/>
+      <c r="P95" s="10"/>
+      <c r="Q95" s="10"/>
+      <c r="R95" s="10"/>
+      <c r="S95" s="10"/>
+      <c r="T95" s="10">
+        <v>887</v>
+      </c>
+      <c r="U95" s="12">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="96" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O96" s="11"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="10"/>
+      <c r="R96" s="10"/>
+      <c r="S96" s="10"/>
+      <c r="T96" s="10">
+        <v>909</v>
+      </c>
+      <c r="U96" s="12">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="97" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O97" s="11"/>
+      <c r="P97" s="10"/>
+      <c r="Q97" s="10"/>
+      <c r="R97" s="10"/>
+      <c r="S97" s="10"/>
+      <c r="T97" s="10">
+        <v>931</v>
+      </c>
+      <c r="U97" s="12">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="98" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O98" s="11"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="10"/>
+      <c r="R98" s="10"/>
+      <c r="S98" s="10"/>
+      <c r="T98" s="10">
+        <v>953</v>
+      </c>
+      <c r="U98" s="12">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="99" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O99" s="11"/>
+      <c r="P99" s="10"/>
+      <c r="Q99" s="10"/>
+      <c r="R99" s="10"/>
+      <c r="S99" s="10"/>
+      <c r="T99" s="10">
+        <v>976</v>
+      </c>
+      <c r="U99" s="12">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="100" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O100" s="11"/>
+      <c r="P100" s="10"/>
+      <c r="Q100" s="10"/>
+      <c r="R100" s="10"/>
+      <c r="S100" s="10"/>
+      <c r="T100" s="10"/>
+      <c r="U100" s="12">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="101" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O101" s="11"/>
+      <c r="P101" s="10"/>
+      <c r="Q101" s="10"/>
+      <c r="R101" s="10"/>
+      <c r="S101" s="10"/>
+      <c r="T101" s="10"/>
+      <c r="U101" s="12">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="102" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O102" s="11"/>
+      <c r="P102" s="10"/>
+      <c r="Q102" s="10"/>
+      <c r="R102" s="10"/>
+      <c r="S102" s="10"/>
+      <c r="T102" s="10"/>
+      <c r="U102" s="12">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="103" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O103" s="11"/>
+      <c r="P103" s="10"/>
+      <c r="Q103" s="10"/>
+      <c r="R103" s="10"/>
+      <c r="S103" s="10"/>
+      <c r="T103" s="10"/>
+      <c r="U103" s="12">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="104" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O104" s="11"/>
+      <c r="P104" s="10"/>
+      <c r="Q104" s="10"/>
+      <c r="R104" s="10"/>
+      <c r="S104" s="10"/>
+      <c r="T104" s="10"/>
+      <c r="U104" s="12">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="105" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O105" s="11"/>
+      <c r="P105" s="10"/>
+      <c r="Q105" s="10"/>
+      <c r="R105" s="10"/>
+      <c r="S105" s="10"/>
+      <c r="T105" s="10"/>
+      <c r="U105" s="12">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="106" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O106" s="11"/>
+      <c r="P106" s="10"/>
+      <c r="Q106" s="10"/>
+      <c r="R106" s="10"/>
+      <c r="S106" s="10"/>
+      <c r="T106" s="10"/>
+      <c r="U106" s="12">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="107" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O107" s="11"/>
+      <c r="P107" s="10"/>
+      <c r="Q107" s="10"/>
+      <c r="R107" s="10"/>
+      <c r="S107" s="10"/>
+      <c r="T107" s="10"/>
+      <c r="U107" s="12">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="108" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O108" s="11"/>
+      <c r="P108" s="10"/>
+      <c r="Q108" s="10"/>
+      <c r="R108" s="10"/>
+      <c r="S108" s="10"/>
+      <c r="T108" s="10"/>
+      <c r="U108" s="12">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="109" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O109" s="11"/>
+      <c r="P109" s="10"/>
+      <c r="Q109" s="10"/>
+      <c r="R109" s="10"/>
+      <c r="S109" s="10"/>
+      <c r="T109" s="10"/>
+      <c r="U109" s="12">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="110" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O110" s="11"/>
+      <c r="P110" s="10"/>
+      <c r="Q110" s="10"/>
+      <c r="R110" s="10"/>
+      <c r="S110" s="10"/>
+      <c r="T110" s="10"/>
+      <c r="U110" s="12">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="111" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O111" s="11"/>
+      <c r="P111" s="10"/>
+      <c r="Q111" s="10"/>
+      <c r="R111" s="10"/>
+      <c r="S111" s="10"/>
+      <c r="T111" s="10"/>
+      <c r="U111" s="12">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="112" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O112" s="11"/>
+      <c r="P112" s="10"/>
+      <c r="Q112" s="10"/>
+      <c r="R112" s="10"/>
+      <c r="S112" s="10"/>
+      <c r="T112" s="10"/>
+      <c r="U112" s="12">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="113" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O113" s="11"/>
+      <c r="P113" s="10"/>
+      <c r="Q113" s="10"/>
+      <c r="R113" s="10"/>
+      <c r="S113" s="10"/>
+      <c r="T113" s="10"/>
+      <c r="U113" s="12">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="114" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O114" s="11"/>
+      <c r="P114" s="10"/>
+      <c r="Q114" s="10"/>
+      <c r="R114" s="10"/>
+      <c r="S114" s="10"/>
+      <c r="T114" s="10"/>
+      <c r="U114" s="12">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="115" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O115" s="11"/>
+      <c r="P115" s="10"/>
+      <c r="Q115" s="10"/>
+      <c r="R115" s="10"/>
+      <c r="S115" s="10"/>
+      <c r="T115" s="10"/>
+      <c r="U115" s="12">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="116" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O116" s="11"/>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="10"/>
+      <c r="R116" s="10"/>
+      <c r="S116" s="10"/>
+      <c r="T116" s="10"/>
+      <c r="U116" s="12">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="117" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O117" s="11"/>
+      <c r="P117" s="10"/>
+      <c r="Q117" s="10"/>
+      <c r="R117" s="10"/>
+      <c r="S117" s="10"/>
+      <c r="T117" s="10"/>
+      <c r="U117" s="12">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="118" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O118" s="11"/>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="10"/>
+      <c r="R118" s="10"/>
+      <c r="S118" s="10"/>
+      <c r="T118" s="10"/>
+      <c r="U118" s="12">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="119" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O119" s="11"/>
+      <c r="P119" s="10"/>
+      <c r="Q119" s="10"/>
+      <c r="R119" s="10"/>
+      <c r="S119" s="10"/>
+      <c r="T119" s="10"/>
+      <c r="U119" s="12">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="120" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O120" s="11"/>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="10"/>
+      <c r="R120" s="10"/>
+      <c r="S120" s="10"/>
+      <c r="T120" s="10"/>
+      <c r="U120" s="12">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="121" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O121" s="11"/>
+      <c r="P121" s="10"/>
+      <c r="Q121" s="10"/>
+      <c r="R121" s="10"/>
+      <c r="S121" s="10"/>
+      <c r="T121" s="10"/>
+      <c r="U121" s="12">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="122" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O122" s="11"/>
+      <c r="P122" s="10"/>
+      <c r="Q122" s="10"/>
+      <c r="R122" s="10"/>
+      <c r="S122" s="10"/>
+      <c r="T122" s="10"/>
+      <c r="U122" s="12">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="123" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O123" s="11"/>
+      <c r="P123" s="10"/>
+      <c r="Q123" s="10"/>
+      <c r="R123" s="10"/>
+      <c r="S123" s="10"/>
+      <c r="T123" s="10"/>
+      <c r="U123" s="12">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="124" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O124" s="11"/>
+      <c r="P124" s="10"/>
+      <c r="Q124" s="10"/>
+      <c r="R124" s="10"/>
+      <c r="S124" s="10"/>
+      <c r="T124" s="10"/>
+      <c r="U124" s="12">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="125" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O125" s="11"/>
+      <c r="P125" s="10"/>
+      <c r="Q125" s="10"/>
+      <c r="R125" s="10"/>
+      <c r="S125" s="10"/>
+      <c r="T125" s="10"/>
+      <c r="U125" s="12">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="126" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O126" s="11"/>
+      <c r="P126" s="10"/>
+      <c r="Q126" s="10"/>
+      <c r="R126" s="10"/>
+      <c r="S126" s="10"/>
+      <c r="T126" s="10"/>
+      <c r="U126" s="12">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="127" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O127" s="11"/>
+      <c r="P127" s="10"/>
+      <c r="Q127" s="10"/>
+      <c r="R127" s="10"/>
+      <c r="S127" s="10"/>
+      <c r="T127" s="10"/>
+      <c r="U127" s="12">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="128" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O128" s="11"/>
+      <c r="P128" s="10"/>
+      <c r="Q128" s="10"/>
+      <c r="R128" s="10"/>
+      <c r="S128" s="10"/>
+      <c r="T128" s="10"/>
+      <c r="U128" s="12">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="129" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O129" s="11"/>
+      <c r="P129" s="10"/>
+      <c r="Q129" s="10"/>
+      <c r="R129" s="10"/>
+      <c r="S129" s="10"/>
+      <c r="T129" s="10"/>
+      <c r="U129" s="12">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="130" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O130" s="11"/>
+      <c r="P130" s="10"/>
+      <c r="Q130" s="10"/>
+      <c r="R130" s="10"/>
+      <c r="S130" s="10"/>
+      <c r="T130" s="10"/>
+      <c r="U130" s="12">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="131" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O131" s="11"/>
+      <c r="P131" s="10"/>
+      <c r="Q131" s="10"/>
+      <c r="R131" s="10"/>
+      <c r="S131" s="10"/>
+      <c r="T131" s="10"/>
+      <c r="U131" s="12">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="132" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O132" s="11"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="10"/>
+      <c r="R132" s="10"/>
+      <c r="S132" s="10"/>
+      <c r="T132" s="10"/>
+      <c r="U132" s="12">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="133" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O133" s="11"/>
+      <c r="P133" s="10"/>
+      <c r="Q133" s="10"/>
+      <c r="R133" s="10"/>
+      <c r="S133" s="10"/>
+      <c r="T133" s="10"/>
+      <c r="U133" s="12">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="134" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O134" s="11"/>
+      <c r="P134" s="10"/>
+      <c r="Q134" s="10"/>
+      <c r="R134" s="10"/>
+      <c r="S134" s="10"/>
+      <c r="T134" s="10"/>
+      <c r="U134" s="12">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="135" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O135" s="11"/>
+      <c r="P135" s="10"/>
+      <c r="Q135" s="10"/>
+      <c r="R135" s="10"/>
+      <c r="S135" s="10"/>
+      <c r="T135" s="10"/>
+      <c r="U135" s="12">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="136" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O136" s="11"/>
+      <c r="P136" s="10"/>
+      <c r="Q136" s="10"/>
+      <c r="R136" s="10"/>
+      <c r="S136" s="10"/>
+      <c r="T136" s="10"/>
+      <c r="U136" s="12">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="137" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O137" s="11"/>
+      <c r="P137" s="10"/>
+      <c r="Q137" s="10"/>
+      <c r="R137" s="10"/>
+      <c r="S137" s="10"/>
+      <c r="T137" s="10"/>
+      <c r="U137" s="12">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="138" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O138" s="11"/>
+      <c r="P138" s="10"/>
+      <c r="Q138" s="10"/>
+      <c r="R138" s="10"/>
+      <c r="S138" s="10"/>
+      <c r="T138" s="10"/>
+      <c r="U138" s="12">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="139" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O139" s="11"/>
+      <c r="P139" s="10"/>
+      <c r="Q139" s="10"/>
+      <c r="R139" s="10"/>
+      <c r="S139" s="10"/>
+      <c r="T139" s="10"/>
+      <c r="U139" s="12">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="140" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O140" s="11"/>
+      <c r="P140" s="10"/>
+      <c r="Q140" s="10"/>
+      <c r="R140" s="10"/>
+      <c r="S140" s="10"/>
+      <c r="T140" s="10"/>
+      <c r="U140" s="12">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="141" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O141" s="11"/>
+      <c r="P141" s="10"/>
+      <c r="Q141" s="10"/>
+      <c r="R141" s="10"/>
+      <c r="S141" s="10"/>
+      <c r="T141" s="10"/>
+      <c r="U141" s="12">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="142" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O142" s="11"/>
+      <c r="P142" s="10"/>
+      <c r="Q142" s="10"/>
+      <c r="R142" s="10"/>
+      <c r="S142" s="10"/>
+      <c r="T142" s="10"/>
+      <c r="U142" s="12">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="143" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O143" s="11"/>
+      <c r="P143" s="10"/>
+      <c r="Q143" s="10"/>
+      <c r="R143" s="10"/>
+      <c r="S143" s="10"/>
+      <c r="T143" s="10"/>
+      <c r="U143" s="12">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="144" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O144" s="11"/>
+      <c r="P144" s="10"/>
+      <c r="Q144" s="10"/>
+      <c r="R144" s="10"/>
+      <c r="S144" s="10"/>
+      <c r="T144" s="10"/>
+      <c r="U144" s="12">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="145" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O145" s="11"/>
+      <c r="P145" s="10"/>
+      <c r="Q145" s="10"/>
+      <c r="R145" s="10"/>
+      <c r="S145" s="10"/>
+      <c r="T145" s="10"/>
+      <c r="U145" s="12">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="146" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O146" s="11"/>
+      <c r="P146" s="10"/>
+      <c r="Q146" s="10"/>
+      <c r="R146" s="10"/>
+      <c r="S146" s="10"/>
+      <c r="T146" s="10"/>
+      <c r="U146" s="12">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="147" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O147" s="11"/>
+      <c r="P147" s="10"/>
+      <c r="Q147" s="10"/>
+      <c r="R147" s="10"/>
+      <c r="S147" s="10"/>
+      <c r="T147" s="10"/>
+      <c r="U147" s="12">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="148" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O148" s="11"/>
+      <c r="P148" s="10"/>
+      <c r="Q148" s="10"/>
+      <c r="R148" s="10"/>
+      <c r="S148" s="10"/>
+      <c r="T148" s="10"/>
+      <c r="U148" s="12">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="149" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O149" s="11"/>
+      <c r="P149" s="10"/>
+      <c r="Q149" s="10"/>
+      <c r="R149" s="10"/>
+      <c r="S149" s="10"/>
+      <c r="T149" s="10"/>
+      <c r="U149" s="12">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="150" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O150" s="11"/>
+      <c r="P150" s="10"/>
+      <c r="Q150" s="10"/>
+      <c r="R150" s="10"/>
+      <c r="S150" s="10"/>
+      <c r="T150" s="10"/>
+      <c r="U150" s="12">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="151" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O151" s="11"/>
+      <c r="P151" s="10"/>
+      <c r="Q151" s="10"/>
+      <c r="R151" s="10"/>
+      <c r="S151" s="10"/>
+      <c r="T151" s="10"/>
+      <c r="U151" s="12">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="152" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O152" s="11"/>
+      <c r="P152" s="10"/>
+      <c r="Q152" s="10"/>
+      <c r="R152" s="10"/>
+      <c r="S152" s="10"/>
+      <c r="T152" s="10"/>
+      <c r="U152" s="12">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="153" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O153" s="11"/>
+      <c r="P153" s="10"/>
+      <c r="Q153" s="10"/>
+      <c r="R153" s="10"/>
+      <c r="S153" s="10"/>
+      <c r="T153" s="10"/>
+      <c r="U153" s="12">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="154" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O154" s="11"/>
+      <c r="P154" s="10"/>
+      <c r="Q154" s="10"/>
+      <c r="R154" s="10"/>
+      <c r="S154" s="10"/>
+      <c r="T154" s="10"/>
+      <c r="U154" s="12">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="155" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O155" s="11"/>
+      <c r="P155" s="10"/>
+      <c r="Q155" s="10"/>
+      <c r="R155" s="10"/>
+      <c r="S155" s="10"/>
+      <c r="T155" s="10"/>
+      <c r="U155" s="12">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="156" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O156" s="11"/>
+      <c r="P156" s="10"/>
+      <c r="Q156" s="10"/>
+      <c r="R156" s="10"/>
+      <c r="S156" s="10"/>
+      <c r="T156" s="10"/>
+      <c r="U156" s="12">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="157" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O157" s="11"/>
+      <c r="P157" s="10"/>
+      <c r="Q157" s="10"/>
+      <c r="R157" s="10"/>
+      <c r="S157" s="10"/>
+      <c r="T157" s="10"/>
+      <c r="U157" s="12">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="158" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O158" s="11"/>
+      <c r="P158" s="10"/>
+      <c r="Q158" s="10"/>
+      <c r="R158" s="10"/>
+      <c r="S158" s="10"/>
+      <c r="T158" s="10"/>
+      <c r="U158" s="12">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="159" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O159" s="11"/>
+      <c r="P159" s="10"/>
+      <c r="Q159" s="10"/>
+      <c r="R159" s="10"/>
+      <c r="S159" s="10"/>
+      <c r="T159" s="10"/>
+      <c r="U159" s="12">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="160" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O160" s="11"/>
+      <c r="P160" s="10"/>
+      <c r="Q160" s="10"/>
+      <c r="R160" s="10"/>
+      <c r="S160" s="10"/>
+      <c r="T160" s="10"/>
+      <c r="U160" s="12">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="161" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O161" s="11"/>
+      <c r="P161" s="10"/>
+      <c r="Q161" s="10"/>
+      <c r="R161" s="10"/>
+      <c r="S161" s="10"/>
+      <c r="T161" s="10"/>
+      <c r="U161" s="12">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="162" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O162" s="11"/>
+      <c r="P162" s="10"/>
+      <c r="Q162" s="10"/>
+      <c r="R162" s="10"/>
+      <c r="S162" s="10"/>
+      <c r="T162" s="10"/>
+      <c r="U162" s="12">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="163" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O163" s="11"/>
+      <c r="P163" s="10"/>
+      <c r="Q163" s="10"/>
+      <c r="R163" s="10"/>
+      <c r="S163" s="10"/>
+      <c r="T163" s="10"/>
+      <c r="U163" s="12">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="164" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O164" s="11"/>
+      <c r="P164" s="10"/>
+      <c r="Q164" s="10"/>
+      <c r="R164" s="10"/>
+      <c r="S164" s="10"/>
+      <c r="T164" s="10"/>
+      <c r="U164" s="12">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="165" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O165" s="11"/>
+      <c r="P165" s="10"/>
+      <c r="Q165" s="10"/>
+      <c r="R165" s="10"/>
+      <c r="S165" s="10"/>
+      <c r="T165" s="10"/>
+      <c r="U165" s="12">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="166" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O166" s="11"/>
+      <c r="P166" s="10"/>
+      <c r="Q166" s="10"/>
+      <c r="R166" s="10"/>
+      <c r="S166" s="10"/>
+      <c r="T166" s="10"/>
+      <c r="U166" s="12">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="167" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O167" s="11"/>
+      <c r="P167" s="10"/>
+      <c r="Q167" s="10"/>
+      <c r="R167" s="10"/>
+      <c r="S167" s="10"/>
+      <c r="T167" s="10"/>
+      <c r="U167" s="12">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="168" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O168" s="11"/>
+      <c r="P168" s="10"/>
+      <c r="Q168" s="10"/>
+      <c r="R168" s="10"/>
+      <c r="S168" s="10"/>
+      <c r="T168" s="10"/>
+      <c r="U168" s="12">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="169" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O169" s="11"/>
+      <c r="P169" s="10"/>
+      <c r="Q169" s="10"/>
+      <c r="R169" s="10"/>
+      <c r="S169" s="10"/>
+      <c r="T169" s="10"/>
+      <c r="U169" s="12">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="170" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O170" s="11"/>
+      <c r="P170" s="10"/>
+      <c r="Q170" s="10"/>
+      <c r="R170" s="10"/>
+      <c r="S170" s="10"/>
+      <c r="T170" s="10"/>
+      <c r="U170" s="12">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="171" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O171" s="11"/>
+      <c r="P171" s="10"/>
+      <c r="Q171" s="10"/>
+      <c r="R171" s="10"/>
+      <c r="S171" s="10"/>
+      <c r="T171" s="10"/>
+      <c r="U171" s="12">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="172" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O172" s="11"/>
+      <c r="P172" s="10"/>
+      <c r="Q172" s="10"/>
+      <c r="R172" s="10"/>
+      <c r="S172" s="10"/>
+      <c r="T172" s="10"/>
+      <c r="U172" s="12">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="173" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O173" s="11"/>
+      <c r="P173" s="10"/>
+      <c r="Q173" s="10"/>
+      <c r="R173" s="10"/>
+      <c r="S173" s="10"/>
+      <c r="T173" s="10"/>
+      <c r="U173" s="12">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="174" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O174" s="11"/>
+      <c r="P174" s="10"/>
+      <c r="Q174" s="10"/>
+      <c r="R174" s="10"/>
+      <c r="S174" s="10"/>
+      <c r="T174" s="10"/>
+      <c r="U174" s="12">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="175" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O175" s="11"/>
+      <c r="P175" s="10"/>
+      <c r="Q175" s="10"/>
+      <c r="R175" s="10"/>
+      <c r="S175" s="10"/>
+      <c r="T175" s="10"/>
+      <c r="U175" s="12">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="176" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O176" s="11"/>
+      <c r="P176" s="10"/>
+      <c r="Q176" s="10"/>
+      <c r="R176" s="10"/>
+      <c r="S176" s="10"/>
+      <c r="T176" s="10"/>
+      <c r="U176" s="12">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="177" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O177" s="11"/>
+      <c r="P177" s="10"/>
+      <c r="Q177" s="10"/>
+      <c r="R177" s="10"/>
+      <c r="S177" s="10"/>
+      <c r="T177" s="10"/>
+      <c r="U177" s="12">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="178" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O178" s="11"/>
+      <c r="P178" s="10"/>
+      <c r="Q178" s="10"/>
+      <c r="R178" s="10"/>
+      <c r="S178" s="10"/>
+      <c r="T178" s="10"/>
+      <c r="U178" s="12">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="179" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O179" s="11"/>
+      <c r="P179" s="10"/>
+      <c r="Q179" s="10"/>
+      <c r="R179" s="10"/>
+      <c r="S179" s="10"/>
+      <c r="T179" s="10"/>
+      <c r="U179" s="12">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="180" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O180" s="11"/>
+      <c r="P180" s="10"/>
+      <c r="Q180" s="10"/>
+      <c r="R180" s="10"/>
+      <c r="S180" s="10"/>
+      <c r="T180" s="10"/>
+      <c r="U180" s="12">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="181" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O181" s="11"/>
+      <c r="P181" s="10"/>
+      <c r="Q181" s="10"/>
+      <c r="R181" s="10"/>
+      <c r="S181" s="10"/>
+      <c r="T181" s="10"/>
+      <c r="U181" s="12">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="182" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O182" s="11"/>
+      <c r="P182" s="10"/>
+      <c r="Q182" s="10"/>
+      <c r="R182" s="10"/>
+      <c r="S182" s="10"/>
+      <c r="T182" s="10"/>
+      <c r="U182" s="12">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="183" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O183" s="11"/>
+      <c r="P183" s="10"/>
+      <c r="Q183" s="10"/>
+      <c r="R183" s="10"/>
+      <c r="S183" s="10"/>
+      <c r="T183" s="10"/>
+      <c r="U183" s="12">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="184" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O184" s="11"/>
+      <c r="P184" s="10"/>
+      <c r="Q184" s="10"/>
+      <c r="R184" s="10"/>
+      <c r="S184" s="10"/>
+      <c r="T184" s="10"/>
+      <c r="U184" s="12">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="185" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O185" s="11"/>
+      <c r="P185" s="10"/>
+      <c r="Q185" s="10"/>
+      <c r="R185" s="10"/>
+      <c r="S185" s="10"/>
+      <c r="T185" s="10"/>
+      <c r="U185" s="12">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="186" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O186" s="11"/>
+      <c r="P186" s="10"/>
+      <c r="Q186" s="10"/>
+      <c r="R186" s="10"/>
+      <c r="S186" s="10"/>
+      <c r="T186" s="10"/>
+      <c r="U186" s="12">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="187" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O187" s="11"/>
+      <c r="P187" s="10"/>
+      <c r="Q187" s="10"/>
+      <c r="R187" s="10"/>
+      <c r="S187" s="10"/>
+      <c r="T187" s="10"/>
+      <c r="U187" s="12">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="188" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O188" s="11"/>
+      <c r="P188" s="10"/>
+      <c r="Q188" s="10"/>
+      <c r="R188" s="10"/>
+      <c r="S188" s="10"/>
+      <c r="T188" s="10"/>
+      <c r="U188" s="12">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="189" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O189" s="11"/>
+      <c r="P189" s="10"/>
+      <c r="Q189" s="10"/>
+      <c r="R189" s="10"/>
+      <c r="S189" s="10"/>
+      <c r="T189" s="10"/>
+      <c r="U189" s="12">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="190" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O190" s="11"/>
+      <c r="P190" s="10"/>
+      <c r="Q190" s="10"/>
+      <c r="R190" s="10"/>
+      <c r="S190" s="10"/>
+      <c r="T190" s="10"/>
+      <c r="U190" s="12">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="191" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O191" s="11"/>
+      <c r="P191" s="10"/>
+      <c r="Q191" s="10"/>
+      <c r="R191" s="10"/>
+      <c r="S191" s="10"/>
+      <c r="T191" s="10"/>
+      <c r="U191" s="12">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="192" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O192" s="11"/>
+      <c r="P192" s="10"/>
+      <c r="Q192" s="10"/>
+      <c r="R192" s="10"/>
+      <c r="S192" s="10"/>
+      <c r="T192" s="10"/>
+      <c r="U192" s="12">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="193" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O193" s="11"/>
+      <c r="P193" s="10"/>
+      <c r="Q193" s="10"/>
+      <c r="R193" s="10"/>
+      <c r="S193" s="10"/>
+      <c r="T193" s="10"/>
+      <c r="U193" s="12">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="194" spans="15:21" ht="18" x14ac:dyDescent="0.25">
+      <c r="O194" s="11"/>
+      <c r="P194" s="10"/>
+      <c r="Q194" s="10"/>
+      <c r="R194" s="10"/>
+      <c r="S194" s="10"/>
+      <c r="T194" s="10"/>
+      <c r="U194" s="12">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="195" spans="15:21" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O195" s="13"/>
+      <c r="P195" s="14"/>
+      <c r="Q195" s="14"/>
+      <c r="R195" s="14"/>
+      <c r="S195" s="14"/>
+      <c r="T195" s="14"/>
+      <c r="U195" s="18">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="196" spans="15:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ID calc based on resistors
</commit_message>
<xml_diff>
--- a/TrackAmplifier2.X/doc/Baudrate calc.xlsx
+++ b/TrackAmplifier2.X/doc/Baudrate calc.xlsx
@@ -4031,7 +4031,7 @@
   <dimension ref="C3:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4048,7 +4048,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="7">
-        <v>4.0960000000000001</v>
+        <v>1.024</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -4068,7 +4068,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="8">
-        <v>5000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
@@ -4076,13 +4076,13 @@
         <v>7</v>
       </c>
       <c r="D5" s="7">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="8">
-        <v>3.0000000000000001E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="D6" s="7">
         <f>((D3-D4)*(D5/32))+ D4</f>
-        <v>2.8159999999999998</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
@@ -4100,14 +4100,14 @@
       </c>
       <c r="D7" s="7">
         <f>D6</f>
-        <v>2.8159999999999998</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="7">
-        <f>G3*G5*G4+2.5</f>
-        <v>2.875</v>
+        <f>G3*G5*G4</f>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
@@ -4126,7 +4126,7 @@
   <dimension ref="B2:U196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="20">
-        <f>S4*10</f>
+        <f t="shared" ref="D8:D55" si="1">S4*10</f>
         <v>1000</v>
       </c>
       <c r="E8" s="20">
@@ -4395,19 +4395,19 @@
         <v>8660</v>
       </c>
       <c r="F8" s="21">
-        <f t="shared" ref="F8:F55" si="1">(5/($D8+$E8))*$D8</f>
+        <f t="shared" ref="F8:F55" si="2">(5/($D8+$E8))*$D8</f>
         <v>0.51759834368530022</v>
       </c>
       <c r="G8" s="20">
-        <f t="shared" ref="G8:G55" si="2">ROUND(($F8/$G$3),0)</f>
+        <f t="shared" ref="G8:G55" si="3">ROUND(($F8/$G$3),0)</f>
         <v>106</v>
       </c>
       <c r="H8" s="20">
-        <f t="shared" ref="H8:H55" si="3">G8-G7</f>
+        <f t="shared" ref="H8:H55" si="4">G8-G7</f>
         <v>9</v>
       </c>
       <c r="I8" s="21">
-        <f t="shared" ref="I8:I55" si="4">(F8-F7)*1000</f>
+        <f t="shared" ref="I8:I55" si="5">(F8-F7)*1000</f>
         <v>43.138520923177325</v>
       </c>
       <c r="J8" s="19">
@@ -4440,7 +4440,7 @@
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="20">
-        <f>S5*10</f>
+        <f t="shared" si="1"/>
         <v>1050</v>
       </c>
       <c r="E9" s="20">
@@ -4448,19 +4448,19 @@
         <v>8250</v>
       </c>
       <c r="F9" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.56451612903225812</v>
       </c>
       <c r="G9" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="H9" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="I9" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>46.917785346957899</v>
       </c>
       <c r="J9" s="19">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="20">
-        <f>S6*10</f>
+        <f t="shared" si="1"/>
         <v>1100</v>
       </c>
       <c r="E10" s="20">
@@ -4501,19 +4501,19 @@
         <v>7870</v>
       </c>
       <c r="F10" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.61315496098104794</v>
       </c>
       <c r="G10" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="H10" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="I10" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>48.638831948789814</v>
       </c>
       <c r="J10" s="19">
@@ -4544,7 +4544,7 @@
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="20">
-        <f>S7*10</f>
+        <f t="shared" si="1"/>
         <v>1150</v>
       </c>
       <c r="E11" s="20">
@@ -4552,19 +4552,19 @@
         <v>7500</v>
       </c>
       <c r="F11" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66473988439306364</v>
       </c>
       <c r="G11" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>136</v>
       </c>
       <c r="H11" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="I11" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51.584923412015705</v>
       </c>
       <c r="J11" s="19">
@@ -4595,7 +4595,7 @@
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20">
-        <f>S8*10</f>
+        <f t="shared" si="1"/>
         <v>1210</v>
       </c>
       <c r="E12" s="20">
@@ -4603,19 +4603,19 @@
         <v>7150</v>
       </c>
       <c r="F12" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.72368421052631571</v>
       </c>
       <c r="G12" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>148</v>
       </c>
       <c r="H12" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="I12" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58.944326133252069</v>
       </c>
       <c r="J12" s="19">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20">
-        <f>S9*10</f>
+        <f t="shared" si="1"/>
         <v>1270</v>
       </c>
       <c r="E13" s="20">
@@ -4654,19 +4654,19 @@
         <v>6810</v>
       </c>
       <c r="F13" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.78589108910891092</v>
       </c>
       <c r="G13" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>161</v>
       </c>
       <c r="H13" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="I13" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62.206878582595216</v>
       </c>
       <c r="J13" s="19">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20">
-        <f>S10*10</f>
+        <f t="shared" si="1"/>
         <v>1330</v>
       </c>
       <c r="E14" s="20">
@@ -4705,19 +4705,19 @@
         <v>6490</v>
       </c>
       <c r="F14" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85038363171355502</v>
       </c>
       <c r="G14" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>174</v>
       </c>
       <c r="H14" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="I14" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64.4925426046441</v>
       </c>
       <c r="J14" s="19">
@@ -4748,7 +4748,7 @@
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="20">
-        <f>S11*10</f>
+        <f t="shared" si="1"/>
         <v>1400</v>
       </c>
       <c r="E15" s="20">
@@ -4756,19 +4756,19 @@
         <v>6190</v>
       </c>
       <c r="F15" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92226613965744408</v>
       </c>
       <c r="G15" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>189</v>
       </c>
       <c r="H15" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="I15" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.882507943889067</v>
       </c>
       <c r="J15" s="19">
@@ -4799,7 +4799,7 @@
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="20">
-        <f>S12*10</f>
+        <f t="shared" si="1"/>
         <v>1470</v>
       </c>
       <c r="E16" s="20">
@@ -4807,19 +4807,19 @@
         <v>5900</v>
       </c>
       <c r="F16" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99728629579375838</v>
       </c>
       <c r="G16" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>204</v>
       </c>
       <c r="H16" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="I16" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.020156136314299</v>
       </c>
       <c r="J16" s="19">
@@ -4848,7 +4848,7 @@
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="20">
-        <f>S13*10</f>
+        <f t="shared" si="1"/>
         <v>1540</v>
       </c>
       <c r="E17" s="20">
@@ -4856,11 +4856,11 @@
         <v>5620</v>
       </c>
       <c r="F17" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0754189944134078</v>
       </c>
       <c r="G17" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>220</v>
       </c>
       <c r="H17" s="20">
@@ -4868,7 +4868,7 @@
         <v>16</v>
       </c>
       <c r="I17" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78.132698619649446</v>
       </c>
       <c r="J17" s="19">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20">
-        <f>S14*10</f>
+        <f t="shared" si="1"/>
         <v>1620</v>
       </c>
       <c r="E18" s="20">
@@ -4905,19 +4905,19 @@
         <v>5360</v>
       </c>
       <c r="F18" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1604584527220629</v>
       </c>
       <c r="G18" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>238</v>
       </c>
       <c r="H18" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="I18" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85.039458308655114</v>
       </c>
       <c r="J18" s="19">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20">
-        <f>S15*10</f>
+        <f t="shared" si="1"/>
         <v>1690</v>
       </c>
       <c r="E19" s="20">
@@ -4954,19 +4954,19 @@
         <v>5110</v>
       </c>
       <c r="F19" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2426470588235294</v>
       </c>
       <c r="G19" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>254</v>
       </c>
       <c r="H19" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I19" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>82.188606101466505</v>
       </c>
       <c r="J19" s="19">
@@ -4995,7 +4995,7 @@
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="20">
-        <f>S16*10</f>
+        <f t="shared" si="1"/>
         <v>1780</v>
       </c>
       <c r="E20" s="20">
@@ -5003,19 +5003,19 @@
         <v>4870</v>
       </c>
       <c r="F20" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3383458646616542</v>
       </c>
       <c r="G20" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>274</v>
       </c>
       <c r="H20" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="I20" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>95.698805838124741</v>
       </c>
       <c r="J20" s="19">
@@ -5044,7 +5044,7 @@
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="20">
-        <f>S17*10</f>
+        <f t="shared" si="1"/>
         <v>1870</v>
       </c>
       <c r="E21" s="20">
@@ -5052,19 +5052,19 @@
         <v>4640</v>
       </c>
       <c r="F21" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4362519201228878</v>
       </c>
       <c r="G21" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>294</v>
       </c>
       <c r="H21" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="I21" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>97.906055461233649</v>
       </c>
       <c r="J21" s="19">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="20">
-        <f>S18*10</f>
+        <f t="shared" si="1"/>
         <v>1960</v>
       </c>
       <c r="E22" s="20">
@@ -5101,19 +5101,19 @@
         <v>4420</v>
       </c>
       <c r="F22" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5360501567398119</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>315</v>
       </c>
       <c r="H22" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="I22" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99.7982366169241</v>
       </c>
       <c r="J22" s="19">
@@ -5142,7 +5142,7 @@
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="20">
-        <f>S19*10</f>
+        <f t="shared" si="1"/>
         <v>2050</v>
       </c>
       <c r="E23" s="20">
@@ -5150,19 +5150,19 @@
         <v>4220</v>
       </c>
       <c r="F23" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.634768740031898</v>
       </c>
       <c r="G23" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>335</v>
       </c>
       <c r="H23" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="I23" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>98.718583292086052</v>
       </c>
       <c r="J23" s="19">
@@ -5191,7 +5191,7 @@
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="20">
-        <f>S20*10</f>
+        <f t="shared" si="1"/>
         <v>2150</v>
       </c>
       <c r="E24" s="20">
@@ -5199,19 +5199,19 @@
         <v>4020</v>
       </c>
       <c r="F24" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7423014586709886</v>
       </c>
       <c r="G24" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>357</v>
       </c>
       <c r="H24" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="I24" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>107.53271863909065</v>
       </c>
       <c r="J24" s="19">
@@ -5240,7 +5240,7 @@
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="20">
-        <f>S21*10</f>
+        <f t="shared" si="1"/>
         <v>2260</v>
       </c>
       <c r="E25" s="20">
@@ -5248,19 +5248,19 @@
         <v>3830</v>
       </c>
       <c r="F25" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8555008210180624</v>
       </c>
       <c r="G25" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>380</v>
       </c>
       <c r="H25" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="I25" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>113.19936234707373</v>
       </c>
       <c r="J25" s="19">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="20">
-        <f>S22*10</f>
+        <f t="shared" si="1"/>
         <v>2370</v>
       </c>
       <c r="E26" s="20">
@@ -5297,19 +5297,19 @@
         <v>3650</v>
       </c>
       <c r="F26" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9684385382059801</v>
       </c>
       <c r="G26" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>403</v>
       </c>
       <c r="H26" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="I26" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>112.93771718791778</v>
       </c>
       <c r="J26" s="19">
@@ -5338,7 +5338,7 @@
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="20">
-        <f>S23*10</f>
+        <f t="shared" si="1"/>
         <v>2490</v>
       </c>
       <c r="E27" s="20">
@@ -5346,19 +5346,19 @@
         <v>3480</v>
       </c>
       <c r="F27" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0854271356783918</v>
       </c>
       <c r="G27" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>427</v>
       </c>
       <c r="H27" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I27" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>116.98859747241164</v>
       </c>
       <c r="J27" s="19">
@@ -5387,7 +5387,7 @@
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="20">
-        <f>S24*10</f>
+        <f t="shared" si="1"/>
         <v>2610</v>
       </c>
       <c r="E28" s="20">
@@ -5395,19 +5395,19 @@
         <v>3320</v>
       </c>
       <c r="F28" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2006745362563236</v>
       </c>
       <c r="G28" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>451</v>
       </c>
       <c r="H28" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I28" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>115.24740057793181</v>
       </c>
       <c r="J28" s="19">
@@ -5434,7 +5434,7 @@
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="20">
-        <f>S25*10</f>
+        <f t="shared" si="1"/>
         <v>2740</v>
       </c>
       <c r="E29" s="20">
@@ -5442,19 +5442,19 @@
         <v>3160</v>
       </c>
       <c r="F29" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3220338983050848</v>
       </c>
       <c r="G29" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>476</v>
       </c>
       <c r="H29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="I29" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>121.35936204876118</v>
       </c>
       <c r="J29" s="19">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="20">
-        <f>S26*10</f>
+        <f t="shared" si="1"/>
         <v>2870</v>
       </c>
       <c r="E30" s="20">
@@ -5489,19 +5489,19 @@
         <v>3010</v>
       </c>
       <c r="F30" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4404761904761902</v>
       </c>
       <c r="G30" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="H30" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I30" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>118.44229217110546</v>
       </c>
       <c r="J30" s="19">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="20">
-        <f>S27*10</f>
+        <f t="shared" si="1"/>
         <v>3010</v>
       </c>
       <c r="E31" s="20">
@@ -5536,19 +5536,19 @@
         <v>2870</v>
       </c>
       <c r="F31" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5595238095238093</v>
       </c>
       <c r="G31" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>524</v>
       </c>
       <c r="H31" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I31" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.04761904761907</v>
       </c>
       <c r="J31" s="19">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="20">
-        <f>S28*10</f>
+        <f t="shared" si="1"/>
         <v>3160</v>
       </c>
       <c r="E32" s="20">
@@ -5583,19 +5583,19 @@
         <v>2740</v>
       </c>
       <c r="F32" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.6779661016949152</v>
       </c>
       <c r="G32" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>548</v>
       </c>
       <c r="H32" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I32" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>118.44229217110592</v>
       </c>
       <c r="J32" s="19">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="20">
-        <f>S29*10</f>
+        <f t="shared" si="1"/>
         <v>3320</v>
       </c>
       <c r="E33" s="20">
@@ -5630,19 +5630,19 @@
         <v>2610</v>
       </c>
       <c r="F33" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.799325463743676</v>
       </c>
       <c r="G33" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>573</v>
       </c>
       <c r="H33" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="I33" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>121.35936204876074</v>
       </c>
       <c r="J33" s="19">
@@ -5669,7 +5669,7 @@
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="20">
-        <f>S30*10</f>
+        <f t="shared" si="1"/>
         <v>3480</v>
       </c>
       <c r="E34" s="20">
@@ -5677,19 +5677,19 @@
         <v>2490</v>
       </c>
       <c r="F34" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9145728643216082</v>
       </c>
       <c r="G34" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>597</v>
       </c>
       <c r="H34" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I34" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>115.24740057793225</v>
       </c>
       <c r="J34" s="19">
@@ -5716,7 +5716,7 @@
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="20">
-        <f>S31*10</f>
+        <f t="shared" si="1"/>
         <v>3650</v>
       </c>
       <c r="E35" s="20">
@@ -5724,19 +5724,19 @@
         <v>2370</v>
       </c>
       <c r="F35" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0315614617940199</v>
       </c>
       <c r="G35" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>621</v>
       </c>
       <c r="H35" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I35" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>116.98859747241164</v>
       </c>
       <c r="J35" s="19">
@@ -5763,7 +5763,7 @@
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="20">
-        <f>S32*10</f>
+        <f t="shared" si="1"/>
         <v>3830</v>
       </c>
       <c r="E36" s="20">
@@ -5771,19 +5771,19 @@
         <v>2260</v>
       </c>
       <c r="F36" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.1444991789819374</v>
       </c>
       <c r="G36" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>644</v>
       </c>
       <c r="H36" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="I36" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>112.93771718791757</v>
       </c>
       <c r="J36" s="19">
@@ -5810,7 +5810,7 @@
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="20">
-        <f>S33*10</f>
+        <f t="shared" si="1"/>
         <v>4020</v>
       </c>
       <c r="E37" s="20">
@@ -5818,19 +5818,19 @@
         <v>2150</v>
       </c>
       <c r="F37" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2576985413290114</v>
       </c>
       <c r="G37" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>667</v>
       </c>
       <c r="H37" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="I37" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>113.19936234707396</v>
       </c>
       <c r="J37" s="19">
@@ -5857,7 +5857,7 @@
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="20">
-        <f>S34*10</f>
+        <f t="shared" si="1"/>
         <v>4220</v>
       </c>
       <c r="E38" s="20">
@@ -5865,19 +5865,19 @@
         <v>2050</v>
       </c>
       <c r="F38" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3652312599681022</v>
       </c>
       <c r="G38" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>689</v>
       </c>
       <c r="H38" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="I38" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>107.53271863909086</v>
       </c>
       <c r="J38" s="19">
@@ -5904,7 +5904,7 @@
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="20">
-        <f>S35*10</f>
+        <f t="shared" si="1"/>
         <v>4420</v>
       </c>
       <c r="E39" s="20">
@@ -5912,19 +5912,19 @@
         <v>1960</v>
       </c>
       <c r="F39" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.4639498432601878</v>
       </c>
       <c r="G39" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>709</v>
       </c>
       <c r="H39" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="I39" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>98.718583292085611</v>
       </c>
       <c r="J39" s="19">
@@ -5951,7 +5951,7 @@
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="20">
-        <f>S36*10</f>
+        <f t="shared" si="1"/>
         <v>4640</v>
       </c>
       <c r="E40" s="20">
@@ -5959,19 +5959,19 @@
         <v>1870</v>
       </c>
       <c r="F40" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.563748079877112</v>
       </c>
       <c r="G40" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="H40" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="I40" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99.7982366169241</v>
       </c>
       <c r="J40" s="19">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="20">
-        <f>S37*10</f>
+        <f t="shared" si="1"/>
         <v>4870</v>
       </c>
       <c r="E41" s="20">
@@ -6006,19 +6006,19 @@
         <v>1780</v>
       </c>
       <c r="F41" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.6616541353383463</v>
       </c>
       <c r="G41" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>750</v>
       </c>
       <c r="H41" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="I41" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>97.906055461234317</v>
       </c>
       <c r="J41" s="19">
@@ -6045,7 +6045,7 @@
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="20">
-        <f>S38*10</f>
+        <f t="shared" si="1"/>
         <v>5110</v>
       </c>
       <c r="E42" s="20">
@@ -6053,19 +6053,19 @@
         <v>1690</v>
       </c>
       <c r="F42" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.7573529411764706</v>
       </c>
       <c r="G42" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>770</v>
       </c>
       <c r="H42" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="I42" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>95.698805838124287</v>
       </c>
       <c r="J42" s="19">
@@ -6092,7 +6092,7 @@
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="20">
-        <f>S39*10</f>
+        <f t="shared" si="1"/>
         <v>5360</v>
       </c>
       <c r="E43" s="20">
@@ -6100,19 +6100,19 @@
         <v>1620</v>
       </c>
       <c r="F43" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8395415472779368</v>
       </c>
       <c r="G43" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>786</v>
       </c>
       <c r="H43" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I43" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>82.188606101466277</v>
       </c>
       <c r="J43" s="19">
@@ -6139,7 +6139,7 @@
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="20">
-        <f>S40*10</f>
+        <f t="shared" si="1"/>
         <v>5620</v>
       </c>
       <c r="E44" s="20">
@@ -6147,19 +6147,19 @@
         <v>1540</v>
       </c>
       <c r="F44" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.9245810055865924</v>
       </c>
       <c r="G44" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>804</v>
       </c>
       <c r="H44" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="I44" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85.039458308655554</v>
       </c>
       <c r="J44" s="19">
@@ -6186,7 +6186,7 @@
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="20">
-        <f>S41*10</f>
+        <f t="shared" si="1"/>
         <v>5900</v>
       </c>
       <c r="E45" s="20">
@@ -6194,19 +6194,19 @@
         <v>1470</v>
       </c>
       <c r="F45" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0027137042062408</v>
       </c>
       <c r="G45" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>820</v>
       </c>
       <c r="H45" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="I45" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78.132698619648437</v>
       </c>
       <c r="J45" s="19">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="20">
-        <f>S42*10</f>
+        <f t="shared" si="1"/>
         <v>6190</v>
       </c>
       <c r="E46" s="20">
@@ -6241,19 +6241,19 @@
         <v>1400</v>
       </c>
       <c r="F46" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0777338603425566</v>
       </c>
       <c r="G46" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>835</v>
       </c>
       <c r="H46" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="I46" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.020156136315734</v>
       </c>
       <c r="J46" s="19">
@@ -6280,7 +6280,7 @@
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="20">
-        <f>S43*10</f>
+        <f t="shared" si="1"/>
         <v>6490</v>
       </c>
       <c r="E47" s="20">
@@ -6288,19 +6288,19 @@
         <v>1330</v>
       </c>
       <c r="F47" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.1496163682864458</v>
       </c>
       <c r="G47" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>850</v>
       </c>
       <c r="H47" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="I47" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.882507943889181</v>
       </c>
       <c r="J47" s="19">
@@ -6327,7 +6327,7 @@
       </c>
       <c r="C48" s="19"/>
       <c r="D48" s="20">
-        <f>S44*10</f>
+        <f t="shared" si="1"/>
         <v>6810</v>
       </c>
       <c r="E48" s="20">
@@ -6335,19 +6335,19 @@
         <v>1270</v>
       </c>
       <c r="F48" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.2141089108910892</v>
       </c>
       <c r="G48" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>863</v>
       </c>
       <c r="H48" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="I48" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>64.492542604643432</v>
       </c>
       <c r="J48" s="19">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="20">
-        <f>S45*10</f>
+        <f t="shared" si="1"/>
         <v>7150</v>
       </c>
       <c r="E49" s="20">
@@ -6382,19 +6382,19 @@
         <v>1210</v>
       </c>
       <c r="F49" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.2763157894736841</v>
       </c>
       <c r="G49" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>876</v>
       </c>
       <c r="H49" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="I49" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>62.206878582594882</v>
       </c>
       <c r="J49" s="19">
@@ -6421,7 +6421,7 @@
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="20">
-        <f>S46*10</f>
+        <f t="shared" si="1"/>
         <v>7500</v>
       </c>
       <c r="E50" s="20">
@@ -6429,19 +6429,19 @@
         <v>1150</v>
       </c>
       <c r="F50" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.3352601156069364</v>
       </c>
       <c r="G50" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>888</v>
       </c>
       <c r="H50" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="I50" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>58.944326133252289</v>
       </c>
       <c r="J50" s="19">
@@ -6468,7 +6468,7 @@
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="20">
-        <f>S47*10</f>
+        <f t="shared" si="1"/>
         <v>7870</v>
       </c>
       <c r="E51" s="20">
@@ -6476,19 +6476,19 @@
         <v>1100</v>
       </c>
       <c r="F51" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.3868450390189517</v>
       </c>
       <c r="G51" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>898</v>
       </c>
       <c r="H51" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="I51" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51.584923412015371</v>
       </c>
       <c r="J51" s="19">
@@ -6515,7 +6515,7 @@
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="20">
-        <f>S48*10</f>
+        <f t="shared" si="1"/>
         <v>8250</v>
       </c>
       <c r="E52" s="20">
@@ -6523,19 +6523,19 @@
         <v>1050</v>
       </c>
       <c r="F52" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.435483870967742</v>
       </c>
       <c r="G52" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>908</v>
       </c>
       <c r="H52" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="I52" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>48.638831948790262</v>
       </c>
       <c r="J52" s="19">
@@ -6560,7 +6560,7 @@
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="20">
-        <f>S49*10</f>
+        <f t="shared" si="1"/>
         <v>8660</v>
       </c>
       <c r="E53" s="20">
@@ -6568,19 +6568,19 @@
         <v>1000</v>
       </c>
       <c r="F53" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.4824016563146998</v>
       </c>
       <c r="G53" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>918</v>
       </c>
       <c r="H53" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="I53" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>46.917785346957785</v>
       </c>
       <c r="J53" s="19">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="20">
-        <f>S50*10</f>
+        <f t="shared" si="1"/>
         <v>9090</v>
       </c>
       <c r="E54" s="20">
@@ -6613,11 +6613,11 @@
         <v>953</v>
       </c>
       <c r="F54" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5255401772378772</v>
       </c>
       <c r="G54" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>927</v>
       </c>
       <c r="H54" s="20">
@@ -6625,7 +6625,7 @@
         <v>9</v>
       </c>
       <c r="I54" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43.138520923177381</v>
       </c>
       <c r="J54" s="19">
@@ -6650,7 +6650,7 @@
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="20">
-        <f>S51*10</f>
+        <f t="shared" si="1"/>
         <v>9530</v>
       </c>
       <c r="E55" s="20">
@@ -6658,19 +6658,19 @@
         <v>909</v>
       </c>
       <c r="F55" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5646134687230582</v>
       </c>
       <c r="G55" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>935</v>
       </c>
       <c r="H55" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="I55" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>39.073291485181016</v>
       </c>
       <c r="J55" s="19">

</xml_diff>